<commit_message>
055 Week 11 Update
</commit_message>
<xml_diff>
--- a/data/latest_data_prev.xlsx
+++ b/data/latest_data_prev.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="4YHRzoWSJn+87aclEoF1z+gUwQ4ribwIq3Hh1cnJmFM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="g4vivuFF5Fza6ehFYcyM5HyF+YEY4mv8i2zsL4Yb3FY="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="159">
   <si>
     <t>MARLOW DUKES 2025</t>
   </si>
@@ -219,7 +219,7 @@
     <t>TUNDE</t>
   </si>
   <si>
-    <t>STEVE P</t>
+    <t>TOY BOY</t>
   </si>
   <si>
     <t>DOM</t>
@@ -228,7 +228,7 @@
     <t>BANKSY</t>
   </si>
   <si>
-    <t>MATT B</t>
+    <t>KRYTON</t>
   </si>
   <si>
     <t>CAPTAIN KIRK</t>
@@ -357,7 +357,13 @@
     <t>MAMAS</t>
   </si>
   <si>
+    <t>MATT B</t>
+  </si>
+  <si>
     <t>BAZ</t>
+  </si>
+  <si>
+    <t>STEVE P</t>
   </si>
   <si>
     <t>WK 50</t>
@@ -792,10 +798,10 @@
     <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2211,7 +2217,7 @@
       <c r="BG11" s="20"/>
     </row>
     <row r="12">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>66</v>
       </c>
       <c r="B12" s="26"/>
@@ -2307,7 +2313,7 @@
       <c r="BG12" s="20"/>
     </row>
     <row r="13">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="26"/>
@@ -2493,7 +2499,7 @@
       <c r="BG14" s="20"/>
     </row>
     <row r="15">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>69</v>
       </c>
       <c r="B15" s="26"/>
@@ -2589,7 +2595,7 @@
       <c r="BG15" s="20"/>
     </row>
     <row r="16">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="36" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="26"/>
@@ -2685,7 +2691,7 @@
       <c r="BG16" s="20"/>
     </row>
     <row r="17">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>71</v>
       </c>
       <c r="B17" s="26"/>
@@ -2783,7 +2789,7 @@
       <c r="BG17" s="20"/>
     </row>
     <row r="18">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="36" t="s">
         <v>72</v>
       </c>
       <c r="B18" s="26"/>
@@ -2881,7 +2887,7 @@
       <c r="BG18" s="20"/>
     </row>
     <row r="19">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>73</v>
       </c>
       <c r="B19" s="26"/>
@@ -2979,7 +2985,7 @@
       <c r="BG19" s="20"/>
     </row>
     <row r="20">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="36" t="s">
         <v>74</v>
       </c>
       <c r="B20" s="26"/>
@@ -3069,7 +3075,7 @@
       <c r="BG20" s="20"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="36" t="s">
         <v>75</v>
       </c>
       <c r="B21" s="26"/>
@@ -3165,7 +3171,7 @@
       <c r="BG21" s="20"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B22" s="26"/>
@@ -3263,7 +3269,7 @@
       <c r="BG22" s="20"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="36" t="s">
         <v>77</v>
       </c>
       <c r="B23" s="26"/>
@@ -3361,7 +3367,7 @@
       <c r="BG23" s="20"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="36" t="s">
         <v>78</v>
       </c>
       <c r="B24" s="26"/>
@@ -3449,7 +3455,7 @@
       <c r="BG24" s="20"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="36" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="26"/>
@@ -3541,7 +3547,7 @@
       <c r="BG25" s="20"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="36" t="s">
         <v>80</v>
       </c>
       <c r="B26" s="26"/>
@@ -3631,7 +3637,7 @@
       <c r="BG26" s="20"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="36" t="s">
         <v>81</v>
       </c>
       <c r="B27" s="26"/>
@@ -3725,7 +3731,7 @@
       <c r="BG27" s="20"/>
     </row>
     <row r="28">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="36" t="s">
         <v>82</v>
       </c>
       <c r="B28" s="26"/>
@@ -3899,7 +3905,7 @@
       <c r="BG29" s="20"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="36" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="26"/>
@@ -3985,7 +3991,7 @@
       <c r="BG30" s="20"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="36" t="s">
         <v>85</v>
       </c>
       <c r="B31" s="26"/>
@@ -4071,7 +4077,7 @@
       <c r="BG31" s="20"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="36" t="s">
         <v>86</v>
       </c>
       <c r="B32" s="26"/>
@@ -4157,7 +4163,7 @@
       <c r="BG32" s="20"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="36" t="s">
         <v>87</v>
       </c>
       <c r="B33" s="26"/>
@@ -4243,7 +4249,7 @@
       <c r="BG33" s="20"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="36" t="s">
         <v>88</v>
       </c>
       <c r="B34" s="26"/>
@@ -4329,7 +4335,7 @@
       <c r="BG34" s="20"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="36" t="s">
         <v>89</v>
       </c>
       <c r="B35" s="26"/>
@@ -4415,7 +4421,7 @@
       <c r="BG35" s="20"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="36" t="s">
         <v>90</v>
       </c>
       <c r="B36" s="26"/>
@@ -4501,7 +4507,7 @@
       <c r="BG36" s="20"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="36" t="s">
         <v>91</v>
       </c>
       <c r="B37" s="26"/>
@@ -4587,7 +4593,7 @@
       <c r="BG37" s="20"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="36" t="s">
         <v>92</v>
       </c>
       <c r="B38" s="26"/>
@@ -4673,7 +4679,7 @@
       <c r="BG38" s="20"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="36" t="s">
         <v>93</v>
       </c>
       <c r="B39" s="26"/>
@@ -4763,7 +4769,7 @@
       <c r="BG39" s="20"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="36" t="s">
         <v>94</v>
       </c>
       <c r="B40" s="26"/>
@@ -25722,7 +25728,7 @@
       <c r="J8" s="46"/>
     </row>
     <row r="9">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>110</v>
       </c>
       <c r="B9" s="44">
@@ -25747,7 +25753,7 @@
       <c r="J9" s="46"/>
     </row>
     <row r="10">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="36" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="44">
@@ -25773,7 +25779,7 @@
       <c r="J10" s="46"/>
     </row>
     <row r="11">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="36" t="s">
         <v>63</v>
       </c>
       <c r="B11" s="44">
@@ -25798,7 +25804,7 @@
       <c r="J11" s="46"/>
     </row>
     <row r="12">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="44">
@@ -25829,7 +25835,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="44">
@@ -25861,7 +25867,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="36" t="s">
         <v>76</v>
       </c>
       <c r="G14" s="44">
@@ -25877,7 +25883,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>81</v>
       </c>
       <c r="G15" s="44">
@@ -25893,7 +25899,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="36" t="s">
         <v>80</v>
       </c>
       <c r="G16" s="44">
@@ -25909,7 +25915,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>66</v>
       </c>
       <c r="G17" s="44">
@@ -25925,7 +25931,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="36" t="s">
         <v>60</v>
       </c>
       <c r="G18" s="44">
@@ -25941,7 +25947,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>74</v>
       </c>
       <c r="G19" s="44">
@@ -25957,7 +25963,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="36" t="s">
         <v>70</v>
       </c>
       <c r="G20" s="44">
@@ -25973,8 +25979,8 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="35" t="s">
-        <v>68</v>
+      <c r="A21" s="36" t="s">
+        <v>111</v>
       </c>
       <c r="G21" s="44">
         <f t="shared" si="1"/>
@@ -25989,7 +25995,7 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="36" t="s">
         <v>88</v>
       </c>
       <c r="G22" s="44">
@@ -26005,7 +26011,7 @@
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="36" t="s">
         <v>93</v>
       </c>
       <c r="G23" s="44">
@@ -26021,7 +26027,7 @@
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="36" t="s">
         <v>89</v>
       </c>
       <c r="G24" s="44">
@@ -26037,7 +26043,7 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="36" t="s">
         <v>94</v>
       </c>
       <c r="G25" s="44">
@@ -26053,7 +26059,7 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="36" t="s">
         <v>92</v>
       </c>
       <c r="G26" s="44">
@@ -26069,7 +26075,7 @@
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="36" t="s">
         <v>91</v>
       </c>
       <c r="G27" s="44">
@@ -26081,7 +26087,7 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="36" t="s">
         <v>87</v>
       </c>
       <c r="G28" s="44">
@@ -26093,8 +26099,8 @@
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="35" t="s">
-        <v>111</v>
+      <c r="A29" s="36" t="s">
+        <v>112</v>
       </c>
       <c r="G29" s="44">
         <f t="shared" si="1"/>
@@ -26105,7 +26111,7 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="36" t="s">
         <v>85</v>
       </c>
       <c r="G30" s="44">
@@ -26117,7 +26123,7 @@
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="36" t="s">
         <v>78</v>
       </c>
       <c r="G31" s="44">
@@ -26129,7 +26135,7 @@
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="36" t="s">
         <v>86</v>
       </c>
       <c r="G32" s="44">
@@ -26138,7 +26144,7 @@
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="36" t="s">
         <v>90</v>
       </c>
       <c r="G33" s="44">
@@ -26147,7 +26153,7 @@
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="36" t="s">
         <v>84</v>
       </c>
       <c r="G34" s="44">
@@ -26156,8 +26162,8 @@
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="35" t="s">
-        <v>65</v>
+      <c r="A35" s="36" t="s">
+        <v>113</v>
       </c>
       <c r="G35" s="44">
         <f t="shared" si="1"/>
@@ -27313,17 +27319,17 @@
         <v>50</v>
       </c>
       <c r="AY1" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="BB1" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="BC1" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2">
@@ -27702,7 +27708,7 @@
     </row>
     <row r="8">
       <c r="A8" s="30" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -27767,8 +27773,8 @@
       <c r="BC8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="35" t="s">
-        <v>65</v>
+      <c r="A9" s="36" t="s">
+        <v>113</v>
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="28">
@@ -27833,7 +27839,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="36" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="28"/>
@@ -27899,7 +27905,7 @@
       <c r="BC10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="36" t="s">
         <v>63</v>
       </c>
       <c r="B11" s="28"/>
@@ -27965,7 +27971,7 @@
       <c r="BC11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="28"/>
@@ -28032,7 +28038,7 @@
       <c r="BF12" s="6"/>
     </row>
     <row r="13">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="28"/>
@@ -28096,7 +28102,7 @@
       <c r="BC13" s="5"/>
     </row>
     <row r="14">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="36" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="28"/>
@@ -28160,7 +28166,7 @@
       <c r="BC14" s="5"/>
     </row>
     <row r="15">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>79</v>
       </c>
       <c r="B15" s="28"/>
@@ -28224,7 +28230,7 @@
       <c r="BC15" s="5"/>
     </row>
     <row r="16">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="36" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="28"/>
@@ -28288,7 +28294,7 @@
       <c r="BC16" s="5"/>
     </row>
     <row r="17">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>80</v>
       </c>
       <c r="B17" s="28"/>
@@ -28352,7 +28358,7 @@
       <c r="BC17" s="5"/>
     </row>
     <row r="18">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="36" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="28"/>
@@ -28417,7 +28423,7 @@
       <c r="BF18" s="6"/>
     </row>
     <row r="19">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B19" s="28"/>
@@ -28481,7 +28487,7 @@
       <c r="BC19" s="5"/>
     </row>
     <row r="20">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="36" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="28"/>
@@ -28545,7 +28551,7 @@
       <c r="BC20" s="5"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="36" t="s">
         <v>91</v>
       </c>
       <c r="B21" s="28"/>
@@ -28609,7 +28615,7 @@
       <c r="BC21" s="5"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="36" t="s">
         <v>59</v>
       </c>
       <c r="B22" s="28"/>
@@ -28671,7 +28677,7 @@
       <c r="BC22" s="5"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="36" t="s">
         <v>75</v>
       </c>
       <c r="B23" s="28"/>
@@ -28733,7 +28739,7 @@
       <c r="BC23" s="5"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="36" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="28"/>
@@ -28795,7 +28801,7 @@
       <c r="BC24" s="5"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="36" t="s">
         <v>93</v>
       </c>
       <c r="B25" s="28"/>
@@ -28857,7 +28863,7 @@
       <c r="BC25" s="5"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="36" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="28"/>
@@ -28919,8 +28925,8 @@
       <c r="BC26" s="5"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="35" t="s">
-        <v>111</v>
+      <c r="A27" s="36" t="s">
+        <v>112</v>
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
@@ -28981,7 +28987,7 @@
       <c r="BC27" s="5"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="36" t="s">
         <v>74</v>
       </c>
       <c r="B28" s="28"/>
@@ -29043,7 +29049,7 @@
       <c r="BC28" s="5"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="36" t="s">
         <v>89</v>
       </c>
       <c r="B29" s="28"/>
@@ -29105,7 +29111,7 @@
       <c r="BC29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="36" t="s">
         <v>78</v>
       </c>
       <c r="B30" s="28"/>
@@ -29167,7 +29173,7 @@
       <c r="BC30" s="5"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="36" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="28"/>
@@ -29229,7 +29235,7 @@
       <c r="BC31" s="5"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="36" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="28"/>
@@ -29291,7 +29297,7 @@
       <c r="BC32" s="5"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="36" t="s">
         <v>88</v>
       </c>
       <c r="B33" s="28"/>
@@ -29353,7 +29359,7 @@
       <c r="BC33" s="5"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="36" t="s">
         <v>90</v>
       </c>
       <c r="B34" s="28"/>
@@ -29415,7 +29421,7 @@
       <c r="BC34" s="5"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="36" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="28"/>
@@ -29477,7 +29483,7 @@
       <c r="BC35" s="5"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="36" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="28"/>
@@ -29861,7 +29867,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="44" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B41" s="44">
         <f t="shared" ref="B41:AV41" si="2">SUM(B3:B37)</f>
@@ -60779,7 +60785,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="2"/>
@@ -60944,10 +60950,10 @@
         <v>50</v>
       </c>
       <c r="AY3" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="BA3" s="54" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
@@ -61073,7 +61079,7 @@
     </row>
     <row r="6">
       <c r="A6" s="30" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B6" s="55"/>
       <c r="C6" s="55"/>
@@ -61329,7 +61335,7 @@
     </row>
     <row r="10">
       <c r="A10" s="30" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="28">
@@ -61391,7 +61397,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="36" t="s">
         <v>72</v>
       </c>
       <c r="B11" s="28"/>
@@ -61452,7 +61458,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="32"/>
@@ -61513,7 +61519,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="28"/>
@@ -61574,8 +61580,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="35" t="s">
-        <v>120</v>
+      <c r="A14" s="36" t="s">
+        <v>122</v>
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
@@ -61635,7 +61641,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>93</v>
       </c>
       <c r="B15" s="28"/>
@@ -61696,7 +61702,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="36" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="28"/>
@@ -61757,7 +61763,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>74</v>
       </c>
       <c r="B17" s="28"/>
@@ -61816,7 +61822,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="36" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="28"/>
@@ -61875,7 +61881,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>71</v>
       </c>
       <c r="B19" s="28"/>
@@ -61934,7 +61940,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="36" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="28"/>
@@ -61993,7 +61999,7 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="36" t="s">
         <v>91</v>
       </c>
       <c r="B21" s="28"/>
@@ -62052,7 +62058,7 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="36" t="s">
         <v>92</v>
       </c>
       <c r="B22" s="28"/>
@@ -62111,7 +62117,7 @@
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="36" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="28"/>
@@ -62170,7 +62176,7 @@
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="36" t="s">
         <v>75</v>
       </c>
       <c r="B24" s="28"/>
@@ -62229,7 +62235,7 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="36" t="s">
         <v>86</v>
       </c>
       <c r="B25" s="28"/>
@@ -62288,8 +62294,8 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="35" t="s">
-        <v>121</v>
+      <c r="A26" s="36" t="s">
+        <v>123</v>
       </c>
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
@@ -62347,8 +62353,8 @@
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="35" t="s">
-        <v>68</v>
+      <c r="A27" s="36" t="s">
+        <v>111</v>
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
@@ -62406,7 +62412,7 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="36" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="28"/>
@@ -62465,7 +62471,7 @@
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="36" t="s">
         <v>94</v>
       </c>
       <c r="B29" s="28"/>
@@ -62524,8 +62530,8 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="35" t="s">
-        <v>122</v>
+      <c r="A30" s="36" t="s">
+        <v>124</v>
       </c>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
@@ -62583,7 +62589,7 @@
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="36" t="s">
         <v>88</v>
       </c>
       <c r="B31" s="28"/>
@@ -62642,7 +62648,7 @@
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="36" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="28"/>
@@ -62701,7 +62707,7 @@
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="36" t="s">
         <v>73</v>
       </c>
       <c r="B33" s="28"/>
@@ -62760,7 +62766,7 @@
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="36" t="s">
         <v>78</v>
       </c>
       <c r="B34" s="28"/>
@@ -62819,7 +62825,7 @@
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="36" t="s">
         <v>80</v>
       </c>
       <c r="B35" s="28"/>
@@ -62878,7 +62884,7 @@
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="36" t="s">
         <v>63</v>
       </c>
       <c r="B36" s="28"/>
@@ -62937,7 +62943,7 @@
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="36" t="s">
         <v>90</v>
       </c>
       <c r="B37" s="28"/>
@@ -62996,7 +63002,7 @@
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="35"/>
+      <c r="A38" s="36"/>
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
       <c r="D38" s="28"/>
@@ -63156,7 +63162,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B41" s="5">
         <f t="shared" ref="B41:AY41" si="2">SUM(B5:B39)</f>
@@ -64347,19 +64353,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="44" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -64375,16 +64381,16 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G3" s="50"/>
       <c r="H3" s="5"/>
@@ -64396,10 +64402,10 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50"/>
@@ -64413,16 +64419,16 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G5" s="50"/>
       <c r="H5" s="5"/>
@@ -64434,16 +64440,16 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G6" s="50"/>
       <c r="H6" s="5"/>
@@ -64455,27 +64461,27 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G7" s="50"/>
       <c r="H7" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I7" s="5"/>
       <c r="K7" s="44" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="M7" s="44" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="N7" s="5"/>
     </row>
@@ -64484,16 +64490,16 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="5"/>
@@ -64505,30 +64511,30 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E9" s="50" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I9" s="5">
         <v>2.0</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="N9" s="5">
         <v>2.0</v>
@@ -64544,15 +64550,15 @@
       <c r="E10" s="50"/>
       <c r="G10" s="50"/>
       <c r="H10" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I10" s="5"/>
       <c r="K10" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N10" s="5">
         <v>2.0</v>
@@ -64568,15 +64574,15 @@
       <c r="E11" s="50"/>
       <c r="G11" s="50"/>
       <c r="H11" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="N11" s="5">
         <v>2.0</v>
@@ -64592,15 +64598,15 @@
       <c r="E12" s="50"/>
       <c r="G12" s="50"/>
       <c r="H12" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I12" s="5"/>
       <c r="K12" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="N12" s="5">
         <v>2.0</v>
@@ -64617,15 +64623,15 @@
       <c r="F13" s="50"/>
       <c r="G13" s="50"/>
       <c r="H13" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="N13" s="5">
         <v>1.0</v>
@@ -64641,13 +64647,13 @@
       <c r="E14" s="50"/>
       <c r="G14" s="50"/>
       <c r="H14" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N14" s="5">
         <v>1.0</v>
@@ -64663,13 +64669,13 @@
       <c r="E15" s="50"/>
       <c r="G15" s="50"/>
       <c r="H15" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="I15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="N15" s="5">
         <v>1.0</v>
@@ -64685,13 +64691,13 @@
       <c r="E16" s="60"/>
       <c r="G16" s="50"/>
       <c r="H16" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="N16" s="5">
         <v>1.0</v>
@@ -64707,13 +64713,13 @@
       <c r="E17" s="50"/>
       <c r="G17" s="50"/>
       <c r="H17" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N17" s="5">
         <v>1.0</v>
@@ -64733,7 +64739,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N18" s="5">
         <v>1.0</v>
@@ -64753,7 +64759,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N19" s="5">
         <v>1.0</v>

</xml_diff>

<commit_message>
064 Game week 19 update
</commit_message>
<xml_diff>
--- a/data/latest_data_prev.xlsx
+++ b/data/latest_data_prev.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="6gNUf0hGLVgnOgh7+iO1a49nYPtIhHgVVQWqCdorvyA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="FqOX//pNsjCv6g2IFLN0FKhbvWJmRAzSKTWgJfdfp+o="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="188">
   <si>
     <t>MARLOW DUKES 2025</t>
   </si>
@@ -210,10 +210,10 @@
     <t>KERMIT</t>
   </si>
   <si>
-    <t xml:space="preserve">MAMAS </t>
+    <t>CAPTAIN KIRK</t>
   </si>
   <si>
-    <t>CAPTAIN KIRK</t>
+    <t xml:space="preserve">MAMAS </t>
   </si>
   <si>
     <t>BRUCE</t>
@@ -225,28 +225,28 @@
     <t>CARLOS</t>
   </si>
   <si>
+    <t>INSPECTOR GADGET</t>
+  </si>
+  <si>
+    <t>DWARF</t>
+  </si>
+  <si>
     <t>PRESTON</t>
   </si>
   <si>
-    <t>INSPECTOR GADGET</t>
+    <t>ARTIST</t>
+  </si>
+  <si>
+    <t>FLO</t>
   </si>
   <si>
     <t>DUNCAN</t>
-  </si>
-  <si>
-    <t>DWARF</t>
   </si>
   <si>
     <t>KRYTON</t>
   </si>
   <si>
     <t>ZIGZAG</t>
-  </si>
-  <si>
-    <t>ARTIST</t>
-  </si>
-  <si>
-    <t>FLO</t>
   </si>
   <si>
     <t>TUNDE</t>
@@ -584,6 +584,9 @@
   <si>
     <t>Captain Kirk</t>
   </si>
+  <si>
+    <t>ZigZag - Wilson</t>
+  </si>
 </sst>
 </file>
 
@@ -800,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -931,6 +934,9 @@
     </xf>
     <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -1667,7 +1673,9 @@
       <c r="R5" s="16">
         <v>0.0</v>
       </c>
-      <c r="S5" s="16"/>
+      <c r="S5" s="16">
+        <v>2.0</v>
+      </c>
       <c r="T5" s="16"/>
       <c r="U5" s="16"/>
       <c r="V5" s="16"/>
@@ -1704,11 +1712,11 @@
       </c>
       <c r="AZ5" s="5">
         <f t="shared" ref="AZ5:AZ40" si="1">COUNT(B5:AX5)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA5" s="5">
         <f t="shared" ref="BA5:BA40" si="2">COUNTIF($B5:$AX5, "&gt;=1")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BB5" s="5">
         <f t="shared" ref="BB5:BB40" si="3">COUNTIF($B5:$AX5, "0")</f>
@@ -1720,15 +1728,15 @@
       </c>
       <c r="BD5" s="5">
         <f t="shared" ref="BD5:BD40" si="5">SUM(BA5*3)+BB5</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="BE5" s="5">
         <f t="shared" ref="BE5:BE40" si="6">SUM(B5:AX5)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="BF5" s="20">
         <f t="shared" ref="BF5:BF40" si="7">SUM(BA5*3+BB5*1)/SUM(AZ5*3)</f>
-        <v>0.7435897436</v>
+        <v>0.7619047619</v>
       </c>
       <c r="BG5" s="20"/>
     </row>
@@ -1893,7 +1901,9 @@
       <c r="R7" s="28">
         <v>0.0</v>
       </c>
-      <c r="S7" s="28"/>
+      <c r="S7" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T7" s="28"/>
       <c r="U7" s="28"/>
       <c r="V7" s="28"/>
@@ -1930,7 +1940,7 @@
       </c>
       <c r="AZ7" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA7" s="5">
         <f t="shared" si="2"/>
@@ -1942,7 +1952,7 @@
       </c>
       <c r="BC7" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BD7" s="5">
         <f t="shared" si="5"/>
@@ -1950,11 +1960,11 @@
       </c>
       <c r="BE7" s="5">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="BF7" s="20">
         <f t="shared" si="7"/>
-        <v>0.6666666667</v>
+        <v>0.619047619</v>
       </c>
       <c r="BG7" s="20"/>
     </row>
@@ -1964,7 +1974,7 @@
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="17">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="D8" s="16">
         <v>3.0</v>
@@ -1973,11 +1983,9 @@
         <v>0.0</v>
       </c>
       <c r="F8" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="G8" s="16">
-        <v>3.0</v>
-      </c>
+        <v>-2.0</v>
+      </c>
+      <c r="G8" s="16"/>
       <c r="H8" s="16">
         <v>-3.0</v>
       </c>
@@ -1985,29 +1993,31 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="16">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="16">
         <v>3.0</v>
       </c>
-      <c r="M8" s="16"/>
+      <c r="M8" s="16">
+        <v>1.0</v>
+      </c>
       <c r="N8" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="O8" s="16"/>
+      <c r="P8" s="17">
+        <v>-1.0</v>
+      </c>
+      <c r="Q8" s="16">
         <v>-2.0</v>
       </c>
-      <c r="O8" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="P8" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="Q8" s="16">
+      <c r="R8" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="S8" s="16">
         <v>2.0</v>
       </c>
-      <c r="R8" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="S8" s="16"/>
       <c r="T8" s="16"/>
       <c r="U8" s="16"/>
       <c r="V8" s="16"/>
@@ -2064,7 +2074,7 @@
       </c>
       <c r="BE8" s="5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BF8" s="20">
         <f t="shared" si="7"/>
@@ -2078,7 +2088,7 @@
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="33">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D9" s="34">
         <v>3.0</v>
@@ -2087,9 +2097,11 @@
         <v>0.0</v>
       </c>
       <c r="F9" s="34">
-        <v>-2.0</v>
-      </c>
-      <c r="G9" s="34"/>
+        <v>2.0</v>
+      </c>
+      <c r="G9" s="34">
+        <v>3.0</v>
+      </c>
       <c r="H9" s="34">
         <v>-3.0</v>
       </c>
@@ -2097,29 +2109,31 @@
         <v>2.0</v>
       </c>
       <c r="J9" s="34">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="K9" s="32"/>
       <c r="L9" s="34">
         <v>3.0</v>
       </c>
-      <c r="M9" s="34">
+      <c r="M9" s="34"/>
+      <c r="N9" s="34">
+        <v>-2.0</v>
+      </c>
+      <c r="O9" s="34">
         <v>1.0</v>
       </c>
-      <c r="N9" s="34">
+      <c r="P9" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="Q9" s="34">
         <v>2.0</v>
-      </c>
-      <c r="O9" s="34"/>
-      <c r="P9" s="33">
-        <v>-1.0</v>
-      </c>
-      <c r="Q9" s="34">
-        <v>-2.0</v>
       </c>
       <c r="R9" s="34">
         <v>0.0</v>
       </c>
-      <c r="S9" s="34"/>
+      <c r="S9" s="34">
+        <v>-2.0</v>
+      </c>
       <c r="T9" s="34"/>
       <c r="U9" s="34"/>
       <c r="V9" s="34"/>
@@ -2156,11 +2170,11 @@
       </c>
       <c r="AZ9" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="BA9" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BB9" s="5">
         <f t="shared" si="3"/>
@@ -2168,19 +2182,19 @@
       </c>
       <c r="BC9" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BD9" s="5">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="BE9" s="5">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BF9" s="20">
         <f t="shared" si="7"/>
-        <v>0.5897435897</v>
+        <v>0.5777777778</v>
       </c>
       <c r="BG9" s="20"/>
     </row>
@@ -2233,7 +2247,9 @@
         <v>-2.0</v>
       </c>
       <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
+      <c r="S10" s="34">
+        <v>-2.0</v>
+      </c>
       <c r="T10" s="34"/>
       <c r="U10" s="34"/>
       <c r="V10" s="34"/>
@@ -2270,7 +2286,7 @@
       </c>
       <c r="AZ10" s="5">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BA10" s="5">
         <f t="shared" si="2"/>
@@ -2282,7 +2298,7 @@
       </c>
       <c r="BC10" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="5"/>
@@ -2290,11 +2306,11 @@
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF10" s="20">
         <f t="shared" si="7"/>
-        <v>0.5238095238</v>
+        <v>0.4888888889</v>
       </c>
       <c r="BG10" s="20"/>
     </row>
@@ -2343,7 +2359,9 @@
       <c r="R11" s="28">
         <v>0.0</v>
       </c>
-      <c r="S11" s="28"/>
+      <c r="S11" s="29">
+        <v>2.0</v>
+      </c>
       <c r="T11" s="28"/>
       <c r="U11" s="28"/>
       <c r="V11" s="28"/>
@@ -2380,11 +2398,11 @@
       </c>
       <c r="AZ11" s="5">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BA11" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB11" s="5">
         <f t="shared" si="3"/>
@@ -2396,15 +2414,15 @@
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="BE11" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF11" s="20">
         <f t="shared" si="7"/>
-        <v>0.4722222222</v>
+        <v>0.5128205128</v>
       </c>
       <c r="BG11" s="20"/>
     </row>
@@ -2455,7 +2473,9 @@
       <c r="R12" s="28">
         <v>0.0</v>
       </c>
-      <c r="S12" s="28"/>
+      <c r="S12" s="28">
+        <v>2.0</v>
+      </c>
       <c r="T12" s="28"/>
       <c r="U12" s="28"/>
       <c r="V12" s="28"/>
@@ -2492,11 +2512,11 @@
       </c>
       <c r="AZ12" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA12" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB12" s="5">
         <f t="shared" si="3"/>
@@ -2508,15 +2528,15 @@
       </c>
       <c r="BD12" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="BE12" s="5">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="BF12" s="20">
         <f t="shared" si="7"/>
-        <v>0.4358974359</v>
+        <v>0.4761904762</v>
       </c>
       <c r="BG12" s="20"/>
     </row>
@@ -2526,52 +2546,48 @@
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="29">
-        <v>3.0</v>
-      </c>
-      <c r="E13" s="28">
-        <v>0.0</v>
-      </c>
+        <v>-1.0</v>
+      </c>
+      <c r="D13" s="28">
+        <v>-3.0</v>
+      </c>
+      <c r="E13" s="28"/>
       <c r="F13" s="28">
         <v>-2.0</v>
       </c>
       <c r="G13" s="28">
-        <v>-3.0</v>
-      </c>
-      <c r="H13" s="28">
-        <v>-3.0</v>
-      </c>
+        <v>3.0</v>
+      </c>
+      <c r="H13" s="28"/>
       <c r="I13" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="J13" s="28">
         <v>2.0</v>
       </c>
       <c r="K13" s="27"/>
-      <c r="L13" s="28">
-        <v>-3.0</v>
-      </c>
+      <c r="L13" s="28"/>
       <c r="M13" s="29">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="N13" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="O13" s="28">
         <v>-1.0</v>
       </c>
       <c r="P13" s="28">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q13" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="R13" s="28">
         <v>0.0</v>
       </c>
-      <c r="S13" s="28"/>
+      <c r="S13" s="28">
+        <v>2.0</v>
+      </c>
       <c r="T13" s="28"/>
       <c r="U13" s="28"/>
       <c r="V13" s="28"/>
@@ -2608,31 +2624,31 @@
       </c>
       <c r="AZ13" s="5">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="BA13" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB13" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="BE13" s="5">
         <f t="shared" si="6"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="BF13" s="20">
         <f t="shared" si="7"/>
-        <v>0.3777777778</v>
+        <v>0.4871794872</v>
       </c>
       <c r="BG13" s="20"/>
     </row>
@@ -2648,13 +2664,11 @@
         <v>-3.0</v>
       </c>
       <c r="E14" s="28"/>
-      <c r="F14" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="G14" s="28">
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="29">
         <v>3.0</v>
       </c>
-      <c r="H14" s="28"/>
       <c r="I14" s="28">
         <v>-2.0</v>
       </c>
@@ -2662,26 +2676,28 @@
         <v>2.0</v>
       </c>
       <c r="K14" s="27"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="29">
+      <c r="L14" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="M14" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="N14" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="O14" s="28">
         <v>1.0</v>
       </c>
-      <c r="N14" s="28">
+      <c r="P14" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="Q14" s="28">
         <v>2.0</v>
       </c>
-      <c r="O14" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="P14" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="Q14" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="R14" s="28">
-        <v>0.0</v>
-      </c>
-      <c r="S14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28">
+        <v>2.0</v>
+      </c>
       <c r="T14" s="28"/>
       <c r="U14" s="28"/>
       <c r="V14" s="28"/>
@@ -2722,11 +2738,11 @@
       </c>
       <c r="BA14" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB14" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="5">
         <f t="shared" si="4"/>
@@ -2734,15 +2750,15 @@
       </c>
       <c r="BD14" s="5">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="BE14" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="BF14" s="20">
         <f t="shared" si="7"/>
-        <v>0.4444444444</v>
+        <v>0.5</v>
       </c>
       <c r="BG14" s="20"/>
     </row>
@@ -2752,38 +2768,38 @@
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="D15" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="29">
         <v>3.0</v>
       </c>
       <c r="E15" s="28">
         <v>0.0</v>
       </c>
       <c r="F15" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G15" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="H15" s="28">
         <v>-3.0</v>
       </c>
       <c r="I15" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="J15" s="29">
-        <v>-2.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="J15" s="28">
+        <v>2.0</v>
       </c>
       <c r="K15" s="27"/>
       <c r="L15" s="28">
         <v>-3.0</v>
       </c>
-      <c r="M15" s="28">
+      <c r="M15" s="29">
         <v>-1.0</v>
       </c>
       <c r="N15" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="O15" s="28">
         <v>-1.0</v>
@@ -2794,7 +2810,9 @@
       <c r="Q15" s="28">
         <v>2.0</v>
       </c>
-      <c r="R15" s="28"/>
+      <c r="R15" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S15" s="28"/>
       <c r="T15" s="28"/>
       <c r="U15" s="28"/>
@@ -2832,7 +2850,7 @@
       </c>
       <c r="AZ15" s="5">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BA15" s="5">
         <f t="shared" si="2"/>
@@ -2840,7 +2858,7 @@
       </c>
       <c r="BB15" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC15" s="5">
         <f t="shared" si="4"/>
@@ -2848,15 +2866,15 @@
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BE15" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="BF15" s="20">
         <f t="shared" si="7"/>
-        <v>0.380952381</v>
+        <v>0.3777777778</v>
       </c>
       <c r="BG15" s="20"/>
     </row>
@@ -2865,45 +2883,45 @@
         <v>70</v>
       </c>
       <c r="B16" s="27"/>
-      <c r="C16" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="D16" s="28">
-        <v>-3.0</v>
-      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28">
+        <v>2.0</v>
+      </c>
       <c r="G16" s="28"/>
-      <c r="H16" s="29">
+      <c r="H16" s="28">
         <v>3.0</v>
       </c>
       <c r="I16" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="J16" s="28">
         <v>-2.0</v>
-      </c>
-      <c r="J16" s="28">
-        <v>2.0</v>
       </c>
       <c r="K16" s="27"/>
       <c r="L16" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="M16" s="28">
+        <v>-3.0</v>
+      </c>
+      <c r="M16" s="28"/>
+      <c r="N16" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="O16" s="28">
         <v>-1.0</v>
       </c>
-      <c r="N16" s="28">
+      <c r="P16" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Q16" s="28">
         <v>-2.0</v>
       </c>
-      <c r="O16" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="P16" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="Q16" s="28">
+      <c r="R16" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="S16" s="28">
         <v>2.0</v>
       </c>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
       <c r="T16" s="28"/>
       <c r="U16" s="28"/>
       <c r="V16" s="28"/>
@@ -2948,23 +2966,23 @@
       </c>
       <c r="BB16" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC16" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="BD16" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BE16" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF16" s="20">
         <f t="shared" si="7"/>
-        <v>0.4545454545</v>
+        <v>0.4848484848</v>
       </c>
       <c r="BG16" s="20"/>
     </row>
@@ -2973,9 +2991,11 @@
         <v>71</v>
       </c>
       <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
+      <c r="C17" s="28">
+        <v>1.0</v>
+      </c>
       <c r="D17" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="E17" s="28">
         <v>0.0</v>
@@ -2987,12 +3007,14 @@
       <c r="H17" s="28">
         <v>-3.0</v>
       </c>
-      <c r="I17" s="28">
+      <c r="I17" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="J17" s="28">
         <v>-2.0</v>
       </c>
-      <c r="J17" s="28"/>
       <c r="K17" s="27"/>
-      <c r="L17" s="29">
+      <c r="L17" s="28">
         <v>-3.0</v>
       </c>
       <c r="M17" s="28">
@@ -3000,16 +3022,14 @@
       </c>
       <c r="N17" s="28"/>
       <c r="O17" s="28"/>
-      <c r="P17" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="Q17" s="28">
+      <c r="P17" s="28"/>
+      <c r="Q17" s="29">
         <v>2.0</v>
       </c>
-      <c r="R17" s="28">
-        <v>0.0</v>
-      </c>
-      <c r="S17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28">
+        <v>2.0</v>
+      </c>
       <c r="T17" s="28"/>
       <c r="U17" s="28"/>
       <c r="V17" s="28"/>
@@ -3046,31 +3066,31 @@
       </c>
       <c r="AZ17" s="5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BA17" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB17" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC17" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BE17" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="BF17" s="20">
         <f t="shared" si="7"/>
-        <v>0.4666666667</v>
+        <v>0.4848484848</v>
       </c>
       <c r="BG17" s="20"/>
     </row>
@@ -3085,14 +3105,14 @@
       <c r="D18" s="28">
         <v>3.0</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="28">
         <v>0.0</v>
       </c>
       <c r="F18" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="G18" s="28">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="H18" s="28">
         <v>-3.0</v>
@@ -3100,17 +3120,21 @@
       <c r="I18" s="28">
         <v>-2.0</v>
       </c>
-      <c r="J18" s="28"/>
+      <c r="J18" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="K18" s="27"/>
       <c r="L18" s="28">
         <v>-3.0</v>
       </c>
       <c r="M18" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="N18" s="28"/>
+        <v>-1.0</v>
+      </c>
+      <c r="N18" s="28">
+        <v>2.0</v>
+      </c>
       <c r="O18" s="28">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="P18" s="28">
         <v>-1.0</v>
@@ -3118,9 +3142,7 @@
       <c r="Q18" s="28">
         <v>2.0</v>
       </c>
-      <c r="R18" s="28">
-        <v>0.0</v>
-      </c>
+      <c r="R18" s="28"/>
       <c r="S18" s="28"/>
       <c r="T18" s="28"/>
       <c r="U18" s="28"/>
@@ -3158,31 +3180,31 @@
       </c>
       <c r="AZ18" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA18" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB18" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC18" s="5">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BD18" s="5">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BE18" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>-2</v>
       </c>
       <c r="BF18" s="20">
         <f t="shared" si="7"/>
-        <v>0.358974359</v>
+        <v>0.380952381</v>
       </c>
       <c r="BG18" s="20"/>
     </row>
@@ -3192,37 +3214,37 @@
       </c>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="G19" s="28"/>
+      <c r="D19" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="E19" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28">
+        <v>3.0</v>
+      </c>
       <c r="H19" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I19" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="J19" s="28">
         <v>-2.0</v>
       </c>
+      <c r="J19" s="28"/>
       <c r="K19" s="27"/>
-      <c r="L19" s="28">
+      <c r="L19" s="29">
         <v>-3.0</v>
       </c>
-      <c r="M19" s="28"/>
-      <c r="N19" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="O19" s="28">
+      <c r="M19" s="28">
         <v>-1.0</v>
       </c>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
       <c r="P19" s="28">
         <v>1.0</v>
       </c>
       <c r="Q19" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="R19" s="28">
         <v>0.0</v>
@@ -3272,23 +3294,23 @@
       </c>
       <c r="BB19" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC19" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD19" s="5">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BE19" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="BF19" s="20">
         <f t="shared" si="7"/>
-        <v>0.4333333333</v>
+        <v>0.4666666667</v>
       </c>
       <c r="BG19" s="20"/>
     </row>
@@ -3298,42 +3320,50 @@
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="28">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D20" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="E20" s="29">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="G20" s="28">
         <v>-3.0</v>
-      </c>
-      <c r="E20" s="28">
-        <v>0.0</v>
-      </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28">
-        <v>3.0</v>
       </c>
       <c r="H20" s="28">
         <v>-3.0</v>
       </c>
-      <c r="I20" s="29">
-        <v>2.0</v>
-      </c>
-      <c r="J20" s="28">
+      <c r="I20" s="28">
         <v>-2.0</v>
       </c>
+      <c r="J20" s="28"/>
       <c r="K20" s="27"/>
       <c r="L20" s="28">
         <v>-3.0</v>
       </c>
       <c r="M20" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="P20" s="28">
         <v>-1.0</v>
       </c>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="29">
+      <c r="Q20" s="28">
         <v>2.0</v>
       </c>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
+      <c r="R20" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="S20" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="T20" s="28"/>
       <c r="U20" s="28"/>
       <c r="V20" s="28"/>
@@ -3370,7 +3400,7 @@
       </c>
       <c r="AZ20" s="5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="BA20" s="5">
         <f t="shared" si="2"/>
@@ -3378,23 +3408,23 @@
       </c>
       <c r="BB20" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC20" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-10</v>
       </c>
       <c r="BF20" s="20">
         <f t="shared" si="7"/>
-        <v>0.4333333333</v>
+        <v>0.3333333333</v>
       </c>
       <c r="BG20" s="20"/>
     </row>
@@ -3635,7 +3665,9 @@
       <c r="R23" s="28">
         <v>0.0</v>
       </c>
-      <c r="S23" s="28"/>
+      <c r="S23" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T23" s="28"/>
       <c r="U23" s="28"/>
       <c r="V23" s="28"/>
@@ -3672,7 +3704,7 @@
       </c>
       <c r="AZ23" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA23" s="5">
         <f t="shared" si="2"/>
@@ -3684,7 +3716,7 @@
       </c>
       <c r="BC23" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD23" s="5">
         <f t="shared" si="5"/>
@@ -3692,11 +3724,11 @@
       </c>
       <c r="BE23" s="5">
         <f t="shared" si="6"/>
-        <v>-10</v>
+        <v>-12</v>
       </c>
       <c r="BF23" s="20">
         <f t="shared" si="7"/>
-        <v>0.2820512821</v>
+        <v>0.2619047619</v>
       </c>
       <c r="BG23" s="20"/>
     </row>
@@ -3747,7 +3779,9 @@
       <c r="R24" s="29">
         <v>0.0</v>
       </c>
-      <c r="S24" s="28"/>
+      <c r="S24" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T24" s="28"/>
       <c r="U24" s="28"/>
       <c r="V24" s="28"/>
@@ -3784,7 +3818,7 @@
       </c>
       <c r="AZ24" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA24" s="5">
         <f t="shared" si="2"/>
@@ -3796,7 +3830,7 @@
       </c>
       <c r="BC24" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD24" s="5">
         <f t="shared" si="5"/>
@@ -3804,11 +3838,11 @@
       </c>
       <c r="BE24" s="5">
         <f t="shared" si="6"/>
-        <v>-14</v>
+        <v>-16</v>
       </c>
       <c r="BF24" s="20">
         <f t="shared" si="7"/>
-        <v>0.2820512821</v>
+        <v>0.2619047619</v>
       </c>
       <c r="BG24" s="20"/>
     </row>
@@ -3844,10 +3878,12 @@
       </c>
       <c r="P25" s="28"/>
       <c r="Q25" s="28"/>
-      <c r="R25" s="28">
+      <c r="R25" s="29">
         <v>0.0</v>
       </c>
-      <c r="S25" s="28"/>
+      <c r="S25" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T25" s="28"/>
       <c r="U25" s="28"/>
       <c r="V25" s="28"/>
@@ -3884,7 +3920,7 @@
       </c>
       <c r="AZ25" s="5">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BA25" s="5">
         <f t="shared" si="2"/>
@@ -3896,7 +3932,7 @@
       </c>
       <c r="BC25" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BD25" s="5">
         <f t="shared" si="5"/>
@@ -3904,11 +3940,11 @@
       </c>
       <c r="BE25" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="BF25" s="20">
         <f t="shared" si="7"/>
-        <v>0.380952381</v>
+        <v>0.3333333333</v>
       </c>
       <c r="BG25" s="20"/>
     </row>
@@ -3939,7 +3975,9 @@
         <v>-2.0</v>
       </c>
       <c r="R26" s="28"/>
-      <c r="S26" s="28"/>
+      <c r="S26" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T26" s="28"/>
       <c r="U26" s="28"/>
       <c r="V26" s="28"/>
@@ -3976,7 +4014,7 @@
       </c>
       <c r="AZ26" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BA26" s="5">
         <f t="shared" si="2"/>
@@ -3988,7 +4026,7 @@
       </c>
       <c r="BC26" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BD26" s="5">
         <f t="shared" si="5"/>
@@ -3996,11 +4034,11 @@
       </c>
       <c r="BE26" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="BF26" s="20">
         <f t="shared" si="7"/>
-        <v>0.6666666667</v>
+        <v>0.5</v>
       </c>
       <c r="BG26" s="20"/>
     </row>
@@ -5328,7 +5366,7 @@
       </c>
       <c r="S41" s="34">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T41" s="34">
         <f t="shared" si="8"/>
@@ -25963,7 +26001,7 @@
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="44">
         <v>2.0</v>
@@ -26056,7 +26094,7 @@
     </row>
     <row r="7">
       <c r="A7" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B7" s="45">
         <v>1.0</v>
@@ -26143,7 +26181,7 @@
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B10" s="44">
         <v>2.0</v>
@@ -26168,7 +26206,7 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="44">
         <v>1.0</v>
@@ -26194,7 +26232,7 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="44">
         <v>2.0</v>
@@ -26219,7 +26257,7 @@
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="44">
         <v>2.0</v>
@@ -26234,7 +26272,7 @@
         <v>1.0</v>
       </c>
       <c r="F13" s="44">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="1"/>
@@ -26250,26 +26288,26 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B14" s="44">
+        <v>2.0</v>
+      </c>
+      <c r="C14" s="44">
         <v>1.0</v>
       </c>
-      <c r="C14" s="44">
+      <c r="D14" s="44">
         <v>0.0</v>
       </c>
-      <c r="D14" s="44">
+      <c r="E14" s="44">
         <v>1.0</v>
       </c>
-      <c r="E14" s="44">
-        <v>0.0</v>
-      </c>
       <c r="F14" s="44">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G14" s="44">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="44">
@@ -26277,12 +26315,12 @@
       </c>
       <c r="J14" s="46">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B15" s="44">
         <v>1.0</v>
@@ -26313,7 +26351,7 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B16" s="44">
         <v>2.0</v>
@@ -26328,7 +26366,7 @@
         <v>1.0</v>
       </c>
       <c r="F16" s="44">
-        <v>-3.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G16" s="44">
         <f t="shared" si="1"/>
@@ -26344,38 +26382,38 @@
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="B17" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C17" s="44">
         <v>0.0</v>
       </c>
       <c r="D17" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E17" s="44">
         <v>1.0</v>
       </c>
       <c r="F17" s="44">
-        <v>-1.0</v>
+        <v>-3.0</v>
       </c>
       <c r="G17" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="44">
         <v>23.0</v>
       </c>
       <c r="J17" s="46">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="B18" s="44">
         <v>1.0</v>
@@ -26390,7 +26428,7 @@
         <v>1.0</v>
       </c>
       <c r="F18" s="44">
-        <v>-2.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G18" s="44">
         <f t="shared" si="1"/>
@@ -26406,7 +26444,7 @@
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B19" s="44">
         <v>1.0</v>
@@ -26437,7 +26475,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20" s="44">
         <v>1.0</v>
@@ -26468,7 +26506,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B21" s="44">
         <v>1.0</v>
@@ -27932,14 +27970,51 @@
       <c r="R2" s="7">
         <v>45776.0</v>
       </c>
-      <c r="U2" s="49"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
+      <c r="S2" s="7">
+        <v>45783.0</v>
+      </c>
+      <c r="T2" s="7">
+        <v>45790.0</v>
+      </c>
+      <c r="U2" s="7">
+        <v>45797.0</v>
+      </c>
+      <c r="V2" s="7">
+        <v>45804.0</v>
+      </c>
+      <c r="W2" s="7">
+        <v>45811.0</v>
+      </c>
+      <c r="X2" s="7">
+        <v>45818.0</v>
+      </c>
+      <c r="Y2" s="7">
+        <v>45825.0</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>45832.0</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>45839.0</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>45846.0</v>
+      </c>
+      <c r="AC2" s="7">
+        <v>45853.0</v>
+      </c>
+      <c r="AD2" s="7">
+        <v>45860.0</v>
+      </c>
+      <c r="AE2" s="7">
+        <v>45867.0</v>
+      </c>
+      <c r="AF2" s="7">
+        <v>45874.0</v>
+      </c>
+      <c r="AG2" s="7">
+        <v>45881.0</v>
+      </c>
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
       <c r="AJ2" s="6"/>
@@ -28043,31 +28118,37 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="C4" s="28">
+        <v>2.0</v>
+      </c>
       <c r="D4" s="28">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
-      <c r="G4" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="G4" s="28"/>
       <c r="H4" s="28"/>
-      <c r="I4" s="28">
-        <v>7.0</v>
-      </c>
+      <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="K4" s="27"/>
       <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
+      <c r="M4" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="N4" s="28">
+        <v>1.0</v>
+      </c>
       <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
+      <c r="P4" s="28">
+        <v>1.0</v>
+      </c>
       <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
+      <c r="R4" s="28">
+        <v>1.0</v>
+      </c>
       <c r="S4" s="28"/>
       <c r="T4" s="28"/>
       <c r="U4" s="28"/>
@@ -28104,41 +28185,35 @@
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="BB4" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC4" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="BB4" s="5"/>
+      <c r="BC4" s="5">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B5" s="28"/>
-      <c r="C5" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="C5" s="28"/>
       <c r="D5" s="28">
         <v>1.0</v>
       </c>
       <c r="E5" s="28"/>
-      <c r="F5" s="28">
+      <c r="F5" s="28"/>
+      <c r="G5" s="28">
         <v>1.0</v>
       </c>
-      <c r="G5" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="H5" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="I5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28">
+        <v>7.0</v>
+      </c>
       <c r="J5" s="28"/>
       <c r="K5" s="27"/>
       <c r="L5" s="28"/>
-      <c r="M5" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="M5" s="28"/>
       <c r="N5" s="28"/>
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
@@ -28189,33 +28264,35 @@
     </row>
     <row r="6">
       <c r="A6" s="14" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" s="28">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="F6" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="28">
+        <v>4.0</v>
+      </c>
+      <c r="H6" s="28">
+        <v>1.0</v>
+      </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
       <c r="K6" s="27"/>
       <c r="L6" s="28"/>
       <c r="M6" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="N6" s="28">
         <v>1.0</v>
       </c>
+      <c r="N6" s="28"/>
       <c r="O6" s="28"/>
-      <c r="P6" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="P6" s="28"/>
       <c r="Q6" s="28"/>
       <c r="R6" s="28"/>
       <c r="S6" s="28"/>
@@ -28256,10 +28333,10 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="BB6" s="5"/>
-      <c r="BC6" s="5">
-        <v>3.0</v>
-      </c>
+      <c r="BB6" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="BC6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
@@ -28333,31 +28410,31 @@
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="28"/>
+        <v>73</v>
+      </c>
+      <c r="B8" s="27"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="E8" s="28">
+        <v>2.0</v>
+      </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="28">
+      <c r="G8" s="28"/>
+      <c r="H8" s="28">
         <v>2.0</v>
       </c>
-      <c r="H8" s="28"/>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="27"/>
-      <c r="L8" s="28">
-        <v>3.0</v>
-      </c>
+      <c r="L8" s="28"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
-      <c r="O8" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="O8" s="28"/>
       <c r="P8" s="28"/>
       <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
+      <c r="R8" s="28">
+        <v>2.0</v>
+      </c>
       <c r="S8" s="28"/>
       <c r="T8" s="28"/>
       <c r="U8" s="28"/>
@@ -28397,35 +28474,35 @@
         <v>6</v>
       </c>
       <c r="BB8" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="BC8" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC8" s="5"/>
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28">
-        <v>1.0</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="G9" s="28">
+        <v>2.0</v>
+      </c>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="J9" s="28"/>
       <c r="K9" s="27"/>
-      <c r="L9" s="28"/>
+      <c r="L9" s="28">
+        <v>3.0</v>
+      </c>
       <c r="M9" s="28"/>
-      <c r="N9" s="28">
+      <c r="N9" s="28"/>
+      <c r="O9" s="28">
         <v>1.0</v>
-      </c>
-      <c r="O9" s="28">
-        <v>2.0</v>
       </c>
       <c r="P9" s="28"/>
       <c r="Q9" s="28"/>
@@ -28475,7 +28552,7 @@
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="28">
@@ -28485,22 +28562,22 @@
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="H10" s="28"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K10" s="27"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
+      <c r="N10" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="O10" s="28">
+        <v>2.0</v>
+      </c>
       <c r="P10" s="28"/>
-      <c r="Q10" s="28">
-        <v>3.0</v>
-      </c>
+      <c r="Q10" s="28"/>
       <c r="R10" s="28"/>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
@@ -28547,14 +28624,14 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
+      <c r="C11" s="28">
+        <v>1.0</v>
+      </c>
       <c r="D11" s="28"/>
-      <c r="E11" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="E11" s="28"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28">
@@ -28566,15 +28643,13 @@
       </c>
       <c r="K11" s="27"/>
       <c r="L11" s="28"/>
-      <c r="M11" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="M11" s="28"/>
       <c r="N11" s="28"/>
-      <c r="O11" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="O11" s="28"/>
       <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
+      <c r="Q11" s="28">
+        <v>3.0</v>
+      </c>
       <c r="R11" s="28"/>
       <c r="S11" s="28"/>
       <c r="T11" s="28"/>
@@ -28614,41 +28689,45 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="BB11" s="5"/>
-      <c r="BC11" s="5">
+      <c r="BB11" s="5">
         <v>1.0</v>
       </c>
+      <c r="BC11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="28"/>
-      <c r="D12" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28">
+      <c r="D12" s="28"/>
+      <c r="E12" s="28">
         <v>1.0</v>
       </c>
+      <c r="F12" s="28"/>
       <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
+      <c r="H12" s="28">
+        <v>1.0</v>
+      </c>
       <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
+      <c r="J12" s="28">
+        <v>1.0</v>
+      </c>
       <c r="K12" s="27"/>
       <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28">
+      <c r="M12" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28">
         <v>1.0</v>
       </c>
-      <c r="O12" s="28"/>
       <c r="P12" s="28"/>
       <c r="Q12" s="28"/>
       <c r="R12" s="28"/>
       <c r="S12" s="28"/>
       <c r="T12" s="28"/>
-      <c r="U12" s="50"/>
+      <c r="U12" s="28"/>
       <c r="V12" s="28"/>
       <c r="W12" s="28"/>
       <c r="X12" s="28"/>
@@ -28682,7 +28761,7 @@
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB12" s="5"/>
       <c r="BC12" s="5">
@@ -28692,7 +28771,7 @@
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="28"/>
@@ -28700,23 +28779,23 @@
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
+      <c r="H13" s="28">
+        <v>2.0</v>
+      </c>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
       <c r="K13" s="27"/>
-      <c r="L13" s="28">
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28">
         <v>2.0</v>
       </c>
-      <c r="M13" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="N13" s="28">
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28">
         <v>1.0</v>
       </c>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
       <c r="S13" s="28"/>
       <c r="T13" s="28"/>
       <c r="U13" s="28"/>
@@ -28757,37 +28836,39 @@
       </c>
       <c r="BB13" s="5"/>
       <c r="BC13" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="F14" s="28"/>
+      <c r="D14" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28">
+        <v>1.0</v>
+      </c>
       <c r="G14" s="28"/>
-      <c r="H14" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="27"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
+      <c r="N14" s="28">
+        <v>1.0</v>
+      </c>
       <c r="O14" s="28"/>
       <c r="P14" s="28"/>
       <c r="Q14" s="28"/>
       <c r="R14" s="28"/>
       <c r="S14" s="28"/>
       <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
+      <c r="U14" s="50"/>
       <c r="V14" s="28"/>
       <c r="W14" s="28"/>
       <c r="X14" s="28"/>
@@ -28821,18 +28902,16 @@
       <c r="AZ14" s="6"/>
       <c r="BA14" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="BB14" s="5">
-        <v>1.0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="BB14" s="5"/>
       <c r="BC14" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
@@ -28840,19 +28919,21 @@
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
-      <c r="H15" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="H15" s="28"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
       <c r="K15" s="27"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+      <c r="L15" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="M15" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="N15" s="28">
+        <v>1.0</v>
+      </c>
       <c r="O15" s="28"/>
-      <c r="P15" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="P15" s="28"/>
       <c r="Q15" s="28"/>
       <c r="R15" s="28"/>
       <c r="S15" s="28"/>
@@ -28891,11 +28972,11 @@
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB15" s="5"/>
       <c r="BC15" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -28922,7 +29003,9 @@
       <c r="O16" s="28"/>
       <c r="P16" s="28"/>
       <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
+      <c r="R16" s="28">
+        <v>1.0</v>
+      </c>
       <c r="S16" s="28"/>
       <c r="T16" s="28"/>
       <c r="U16" s="50"/>
@@ -28959,7 +29042,7 @@
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB16" s="5"/>
       <c r="BC16" s="5">
@@ -28994,7 +29077,9 @@
       </c>
       <c r="P17" s="28"/>
       <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
+      <c r="R17" s="28">
+        <v>1.0</v>
+      </c>
       <c r="S17" s="28"/>
       <c r="T17" s="28"/>
       <c r="U17" s="28"/>
@@ -29031,7 +29116,7 @@
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB17" s="5"/>
       <c r="BC17" s="5"/>
@@ -29107,7 +29192,7 @@
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
@@ -29307,7 +29392,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
@@ -29439,7 +29524,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
@@ -29454,12 +29539,14 @@
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
       <c r="N24" s="28"/>
-      <c r="O24" s="28">
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28">
         <v>1.0</v>
       </c>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
+      <c r="R24" s="28">
+        <v>1.0</v>
+      </c>
       <c r="S24" s="28"/>
       <c r="T24" s="28"/>
       <c r="U24" s="28"/>
@@ -29496,22 +29583,18 @@
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BB24" s="5">
-        <v>1.0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="BB24" s="5"/>
       <c r="BC24" s="5"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
-      <c r="D25" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="D25" s="28"/>
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -29522,7 +29605,9 @@
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
       <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
+      <c r="O25" s="28">
+        <v>1.0</v>
+      </c>
       <c r="P25" s="28"/>
       <c r="Q25" s="28"/>
       <c r="R25" s="28"/>
@@ -29564,19 +29649,21 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="BB25" s="5"/>
+      <c r="BB25" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BC25" s="5"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28">
+      <c r="D26" s="28">
         <v>1.0</v>
       </c>
+      <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
@@ -29633,15 +29720,15 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28">
+      <c r="E27" s="28">
         <v>1.0</v>
       </c>
+      <c r="F27" s="28"/>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
@@ -29697,13 +29784,15 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="36" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="B28" s="27"/>
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="F28" s="28">
+        <v>1.0</v>
+      </c>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
@@ -29712,9 +29801,7 @@
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
       <c r="N28" s="28"/>
-      <c r="O28" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="O28" s="28"/>
       <c r="P28" s="28"/>
       <c r="Q28" s="28"/>
       <c r="R28" s="28"/>
@@ -29761,7 +29848,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="28"/>
@@ -29776,11 +29863,11 @@
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
       <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
+      <c r="O29" s="28">
+        <v>1.0</v>
+      </c>
       <c r="P29" s="28"/>
-      <c r="Q29" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="Q29" s="28"/>
       <c r="R29" s="28"/>
       <c r="S29" s="28"/>
       <c r="T29" s="28"/>
@@ -30073,7 +30160,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="27"/>
       <c r="C34" s="28"/>
@@ -30420,7 +30507,7 @@
       </c>
       <c r="S39" s="44">
         <f>'League Table'!S41</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T39" s="44">
         <f>'League Table'!T41</f>
@@ -30648,7 +30735,7 @@
       </c>
       <c r="R41" s="44">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S41" s="44">
         <f t="shared" si="2"/>
@@ -61725,7 +61812,7 @@
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16">
@@ -62021,7 +62108,7 @@
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="34">
@@ -62047,8 +62134,12 @@
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
       <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
+      <c r="R9" s="34">
+        <v>2.0</v>
+      </c>
+      <c r="S9" s="59">
+        <v>2.0</v>
+      </c>
       <c r="T9" s="34"/>
       <c r="U9" s="34"/>
       <c r="V9" s="34"/>
@@ -62083,7 +62174,7 @@
       <c r="AY9" s="34"/>
       <c r="BA9" s="44">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -62222,7 +62313,7 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -62474,7 +62565,7 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -62779,7 +62870,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
@@ -62840,7 +62931,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
@@ -62958,7 +63049,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
@@ -63253,7 +63344,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
@@ -63489,7 +63580,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -64011,11 +64102,11 @@
       </c>
       <c r="R41" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T41" s="5">
         <f t="shared" si="2"/>
@@ -64147,7 +64238,7 @@
       </c>
       <c r="BA41" s="44">
         <f>SUM(B41:AZ41)</f>
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -65319,8 +65410,8 @@
       <c r="M9" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="N9" s="5">
-        <v>3.0</v>
+      <c r="N9" s="60">
+        <v>4.0</v>
       </c>
     </row>
     <row r="10">
@@ -65356,7 +65447,7 @@
         <v>159</v>
       </c>
       <c r="N10" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="11">
@@ -65664,8 +65755,12 @@
       <c r="A20" s="49">
         <v>18.0</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
+      <c r="B20" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>162</v>
+      </c>
       <c r="D20" s="49"/>
       <c r="E20" s="49"/>
       <c r="G20" s="49"/>
@@ -65673,13 +65768,15 @@
         <v>157</v>
       </c>
       <c r="I20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>159</v>
+      </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="N20" s="59">
-        <v>1.0</v>
+        <v>172</v>
+      </c>
+      <c r="N20" s="60">
+        <v>2.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -65698,9 +65795,9 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="N21" s="59">
+        <v>185</v>
+      </c>
+      <c r="N21" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65722,7 +65819,7 @@
       <c r="M22" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="N22" s="59">
+      <c r="N22" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65744,7 +65841,7 @@
       <c r="M23" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="N23" s="59">
+      <c r="N23" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65766,7 +65863,7 @@
       <c r="M24" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N24" s="59">
+      <c r="N24" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65786,7 +65883,7 @@
       <c r="M25" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="N25" s="59">
+      <c r="N25" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65806,7 +65903,7 @@
       <c r="M26" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="N26" s="59">
+      <c r="N26" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65825,7 +65922,7 @@
       <c r="M27" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="N27" s="59">
+      <c r="N27" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65844,7 +65941,7 @@
       <c r="M28" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="N28" s="59">
+      <c r="N28" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65859,8 +65956,6 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="49">
@@ -65979,6 +66074,7 @@
       <c r="E38" s="49"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
+      <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -70883,6 +70979,11 @@
       <c r="H1000" s="5"/>
       <c r="I1000" s="5"/>
       <c r="N1000" s="5"/>
+    </row>
+    <row r="1001" ht="15.75" customHeight="1">
+      <c r="H1001" s="5"/>
+      <c r="I1001" s="5"/>
+      <c r="N1001" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$1:$F$47"/>

</xml_diff>

<commit_message>
070 Game week 26 update
</commit_message>
<xml_diff>
--- a/data/latest_data_prev.xlsx
+++ b/data/latest_data_prev.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="zbNeZnfTuVhrT1fXNsV7QesTSxi4rqtDn/lR/04tpgw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="6p93ohAJ+PXinoAzwzNEgv39A3o0OrLBbQwcA5yoyvk="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="202">
   <si>
     <t>MARLOW DUKES 2025</t>
   </si>
@@ -210,19 +210,13 @@
     <t xml:space="preserve">MAMAS </t>
   </si>
   <si>
+    <t>ZIGZAG</t>
+  </si>
+  <si>
     <t>DOM</t>
   </si>
   <si>
     <t>BRUCE</t>
-  </si>
-  <si>
-    <t>ZIGZAG</t>
-  </si>
-  <si>
-    <t>CAPTAIN KIRK</t>
-  </si>
-  <si>
-    <t>INSPECTOR GADGET</t>
   </si>
   <si>
     <t>DUNCAN</t>
@@ -232,6 +226,12 @@
   </si>
   <si>
     <t>IAN</t>
+  </si>
+  <si>
+    <t>CAPTAIN KIRK</t>
+  </si>
+  <si>
+    <t>INSPECTOR GADGET</t>
   </si>
   <si>
     <t>FATHER TED</t>
@@ -246,10 +246,10 @@
     <t>WILSON</t>
   </si>
   <si>
-    <t>PRESTON</t>
+    <t>FLO</t>
   </si>
   <si>
-    <t>FLO</t>
+    <t>PRESTON</t>
   </si>
   <si>
     <t>TOY BOY</t>
@@ -261,13 +261,16 @@
     <t>TUNDE</t>
   </si>
   <si>
+    <t>SONES</t>
+  </si>
+  <si>
     <t>BANKSY</t>
   </si>
   <si>
-    <t xml:space="preserve">STRAIGHT ROB </t>
+    <t>RYAN</t>
   </si>
   <si>
-    <t>SONES</t>
+    <t xml:space="preserve">STRAIGHT ROB </t>
   </si>
   <si>
     <t>MOO</t>
@@ -279,19 +282,16 @@
     <t>FRED</t>
   </si>
   <si>
+    <t>MICK</t>
+  </si>
+  <si>
+    <t>PHANTOM</t>
+  </si>
+  <si>
     <t>GUEST</t>
   </si>
   <si>
     <t>WOGER</t>
-  </si>
-  <si>
-    <t>RYAN</t>
-  </si>
-  <si>
-    <t>MICK</t>
-  </si>
-  <si>
-    <t>PHANTOM</t>
   </si>
   <si>
     <t>CARZOLA</t>
@@ -306,7 +306,7 @@
     <t>VINCE</t>
   </si>
   <si>
-    <t>JOHN FREWIN</t>
+    <t>KHEN</t>
   </si>
   <si>
     <t># PLAYERS</t>
@@ -357,6 +357,9 @@
     <t xml:space="preserve"> 6-5</t>
   </si>
   <si>
+    <t xml:space="preserve"> 5-3</t>
+  </si>
+  <si>
     <t>P</t>
   </si>
   <si>
@@ -378,13 +381,10 @@
     <t>Ratio</t>
   </si>
   <si>
-    <t>MAMAS</t>
+    <t>SONESY</t>
   </si>
   <si>
-    <t>BAZ</t>
-  </si>
-  <si>
-    <t>GAZZA</t>
+    <t>MAMAS</t>
   </si>
   <si>
     <t>WK 50</t>
@@ -402,6 +402,12 @@
     <t>RICHARD GATER</t>
   </si>
   <si>
+    <t>BAZ</t>
+  </si>
+  <si>
+    <t>CHRIS BRADLEY</t>
+  </si>
+  <si>
     <t># VOTES</t>
   </si>
   <si>
@@ -415,6 +421,9 @@
   </si>
   <si>
     <t>NEW GUY / GUEST</t>
+  </si>
+  <si>
+    <t>GAZZA</t>
   </si>
   <si>
     <t>Total</t>
@@ -504,10 +513,10 @@
     <t>Mamas</t>
   </si>
   <si>
-    <t>Bruce</t>
+    <t>Preston</t>
   </si>
   <si>
-    <t>Preston</t>
+    <t>Bruce</t>
   </si>
   <si>
     <t>Ian - Flo</t>
@@ -552,6 +561,9 @@
     <t>Duncan</t>
   </si>
   <si>
+    <t>Gadget</t>
+  </si>
+  <si>
     <t>Father Ted</t>
   </si>
   <si>
@@ -588,19 +600,16 @@
     <t>ZigZag - Wilson</t>
   </si>
   <si>
-    <t>S Rob</t>
-  </si>
-  <si>
     <t>Carzola - Toy Boy</t>
   </si>
   <si>
     <t>Dwarf</t>
   </si>
   <si>
-    <t>Dom - Kermit</t>
+    <t>S Rob</t>
   </si>
   <si>
-    <t>Gadget</t>
+    <t>Dom - Kermit</t>
   </si>
   <si>
     <t>Gadget - Mamas</t>
@@ -613,6 +622,12 @@
   </si>
   <si>
     <t>Posh - Dwarf</t>
+  </si>
+  <si>
+    <t>Bruce - Sonesy</t>
+  </si>
+  <si>
+    <t>Lost 3-5</t>
   </si>
 </sst>
 </file>
@@ -677,7 +692,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -830,7 +844,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -912,7 +926,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -966,9 +980,6 @@
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1839,7 +1850,9 @@
       <c r="Y6" s="23">
         <v>-1.0</v>
       </c>
-      <c r="Z6" s="23"/>
+      <c r="Z6" s="23">
+        <v>-2.0</v>
+      </c>
       <c r="AA6" s="23"/>
       <c r="AB6" s="23"/>
       <c r="AC6" s="25"/>
@@ -1869,7 +1882,7 @@
       </c>
       <c r="AZ6" s="5">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BA6" s="5">
         <f t="shared" si="2"/>
@@ -1881,7 +1894,7 @@
       </c>
       <c r="BC6" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BD6" s="5">
         <f t="shared" si="5"/>
@@ -1889,11 +1902,11 @@
       </c>
       <c r="BE6" s="5">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BF6" s="20">
         <f t="shared" si="7"/>
-        <v>0.5555555556</v>
+        <v>0.5263157895</v>
       </c>
       <c r="BG6" s="20"/>
     </row>
@@ -2027,63 +2040,69 @@
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="16">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D8" s="16">
-        <v>-3.0</v>
-      </c>
-      <c r="E8" s="16"/>
+        <v>3.0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.0</v>
+      </c>
       <c r="F8" s="16">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G8" s="16">
         <v>-3.0</v>
       </c>
       <c r="H8" s="16">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I8" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="J8" s="17">
-        <v>2.0</v>
-      </c>
+        <v>-2.0</v>
+      </c>
+      <c r="J8" s="16"/>
       <c r="K8" s="15"/>
       <c r="L8" s="16">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="M8" s="16">
         <v>1.0</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="16"/>
+      <c r="O8" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="P8" s="16">
+        <v>-1.0</v>
+      </c>
+      <c r="Q8" s="16">
         <v>2.0</v>
-      </c>
-      <c r="O8" s="16">
-        <v>-1.0</v>
-      </c>
-      <c r="P8" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="Q8" s="16">
-        <v>-2.0</v>
       </c>
       <c r="R8" s="16">
         <v>0.0</v>
       </c>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="17">
+      <c r="S8" s="17">
+        <v>-2.0</v>
+      </c>
+      <c r="T8" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="U8" s="16">
         <v>0.0</v>
       </c>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>1.0</v>
+      </c>
       <c r="W8" s="15"/>
       <c r="X8" s="16">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="Y8" s="16">
-        <v>-1.0</v>
-      </c>
-      <c r="Z8" s="16"/>
+        <v>1.0</v>
+      </c>
+      <c r="Z8" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AA8" s="16"/>
       <c r="AB8" s="16"/>
       <c r="AC8" s="18"/>
@@ -2113,7 +2132,7 @@
       </c>
       <c r="AZ8" s="5">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="BA8" s="5">
         <f t="shared" si="2"/>
@@ -2121,23 +2140,23 @@
       </c>
       <c r="BB8" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BC8" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BD8" s="5">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="BE8" s="5">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="BF8" s="20">
         <f t="shared" si="7"/>
-        <v>0.568627451</v>
+        <v>0.5</v>
       </c>
       <c r="BG8" s="20"/>
     </row>
@@ -2147,14 +2166,12 @@
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="33">
-        <v>-1.0</v>
-      </c>
-      <c r="D9" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="33">
         <v>-3.0</v>
       </c>
-      <c r="E9" s="33">
-        <v>0.0</v>
-      </c>
+      <c r="E9" s="33"/>
       <c r="F9" s="33">
         <v>2.0</v>
       </c>
@@ -2165,9 +2182,9 @@
         <v>3.0</v>
       </c>
       <c r="I9" s="33">
-        <v>-2.0</v>
-      </c>
-      <c r="J9" s="33">
+        <v>2.0</v>
+      </c>
+      <c r="J9" s="34">
         <v>2.0</v>
       </c>
       <c r="K9" s="32"/>
@@ -2180,7 +2197,7 @@
       <c r="N9" s="33">
         <v>2.0</v>
       </c>
-      <c r="O9" s="34">
+      <c r="O9" s="33">
         <v>-1.0</v>
       </c>
       <c r="P9" s="33">
@@ -2189,20 +2206,18 @@
       <c r="Q9" s="33">
         <v>-2.0</v>
       </c>
-      <c r="R9" s="33"/>
-      <c r="S9" s="33">
-        <v>-2.0</v>
-      </c>
-      <c r="T9" s="33">
-        <v>3.0</v>
-      </c>
-      <c r="U9" s="33">
+      <c r="R9" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="34">
         <v>0.0</v>
       </c>
       <c r="V9" s="33"/>
       <c r="W9" s="32"/>
       <c r="X9" s="33">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="Y9" s="33">
         <v>-1.0</v>
@@ -2237,7 +2252,7 @@
       </c>
       <c r="AZ9" s="5">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="BA9" s="5">
         <f t="shared" si="2"/>
@@ -2249,7 +2264,7 @@
       </c>
       <c r="BC9" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="BD9" s="5">
         <f t="shared" si="5"/>
@@ -2257,11 +2272,11 @@
       </c>
       <c r="BE9" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BF9" s="20">
         <f t="shared" si="7"/>
-        <v>0.5087719298</v>
+        <v>0.568627451</v>
       </c>
       <c r="BG9" s="20"/>
     </row>
@@ -2273,46 +2288,48 @@
       <c r="C10" s="33">
         <v>-1.0</v>
       </c>
-      <c r="D10" s="33">
-        <v>3.0</v>
-      </c>
-      <c r="E10" s="34">
+      <c r="D10" s="34">
+        <v>-3.0</v>
+      </c>
+      <c r="E10" s="33">
         <v>0.0</v>
       </c>
       <c r="F10" s="33">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="G10" s="33">
         <v>-3.0</v>
       </c>
       <c r="H10" s="33">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="I10" s="33">
         <v>-2.0</v>
       </c>
-      <c r="J10" s="33"/>
+      <c r="J10" s="33">
+        <v>2.0</v>
+      </c>
       <c r="K10" s="32"/>
       <c r="L10" s="33">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="M10" s="33">
         <v>1.0</v>
       </c>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29">
+      <c r="N10" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="O10" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="P10" s="29">
         <v>1.0</v>
       </c>
-      <c r="P10" s="29">
-        <v>-1.0</v>
-      </c>
       <c r="Q10" s="29">
-        <v>2.0</v>
-      </c>
-      <c r="R10" s="33">
-        <v>0.0</v>
-      </c>
-      <c r="S10" s="34">
+        <v>-2.0</v>
+      </c>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33">
         <v>-2.0</v>
       </c>
       <c r="T10" s="33">
@@ -2321,17 +2338,17 @@
       <c r="U10" s="33">
         <v>0.0</v>
       </c>
-      <c r="V10" s="33">
-        <v>1.0</v>
-      </c>
+      <c r="V10" s="33"/>
       <c r="W10" s="32"/>
       <c r="X10" s="33">
         <v>2.0</v>
       </c>
       <c r="Y10" s="33">
-        <v>1.0</v>
-      </c>
-      <c r="Z10" s="33"/>
+        <v>-1.0</v>
+      </c>
+      <c r="Z10" s="34">
+        <v>-2.0</v>
+      </c>
       <c r="AA10" s="33"/>
       <c r="AB10" s="33"/>
       <c r="AC10" s="35"/>
@@ -2361,31 +2378,31 @@
       </c>
       <c r="AZ10" s="5">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BA10" s="5">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BB10" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BC10" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="BF10" s="20">
         <f t="shared" si="7"/>
-        <v>0.4736842105</v>
+        <v>0.4833333333</v>
       </c>
       <c r="BG10" s="20"/>
     </row>
@@ -2394,8 +2411,8 @@
         <v>65</v>
       </c>
       <c r="B11" s="27"/>
-      <c r="C11" s="28">
-        <v>1.0</v>
+      <c r="C11" s="29">
+        <v>-1.0</v>
       </c>
       <c r="D11" s="29">
         <v>3.0</v>
@@ -2404,48 +2421,60 @@
         <v>0.0</v>
       </c>
       <c r="F11" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="G11" s="29"/>
+        <v>2.0</v>
+      </c>
+      <c r="G11" s="29">
+        <v>3.0</v>
+      </c>
       <c r="H11" s="29">
         <v>-3.0</v>
       </c>
       <c r="I11" s="29">
-        <v>2.0</v>
-      </c>
-      <c r="J11" s="29">
-        <v>2.0</v>
+        <v>-2.0</v>
+      </c>
+      <c r="J11" s="28">
+        <v>-2.0</v>
       </c>
       <c r="K11" s="27"/>
       <c r="L11" s="29">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="M11" s="29">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="N11" s="29">
         <v>2.0</v>
       </c>
-      <c r="O11" s="29"/>
-      <c r="P11" s="28">
+      <c r="O11" s="29">
         <v>-1.0</v>
       </c>
+      <c r="P11" s="29">
+        <v>-1.0</v>
+      </c>
       <c r="Q11" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="R11" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29">
+        <v>-3.0</v>
+      </c>
+      <c r="U11" s="29">
         <v>0.0</v>
       </c>
-      <c r="S11" s="29">
+      <c r="V11" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="W11" s="27"/>
+      <c r="X11" s="28">
         <v>2.0</v>
       </c>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="29"/>
-      <c r="Z11" s="29"/>
+      <c r="Y11" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="Z11" s="29">
+        <v>2.0</v>
+      </c>
       <c r="AA11" s="29"/>
       <c r="AB11" s="29"/>
       <c r="AC11" s="30"/>
@@ -2475,11 +2504,11 @@
       </c>
       <c r="AZ11" s="5">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="BA11" s="5">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BB11" s="5">
         <f t="shared" si="3"/>
@@ -2487,19 +2516,19 @@
       </c>
       <c r="BC11" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="BE11" s="5">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="BF11" s="20">
         <f t="shared" si="7"/>
-        <v>0.619047619</v>
+        <v>0.4833333333</v>
       </c>
       <c r="BG11" s="20"/>
     </row>
@@ -2515,13 +2544,11 @@
         <v>-3.0</v>
       </c>
       <c r="E12" s="29"/>
-      <c r="F12" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="G12" s="29">
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="28">
         <v>3.0</v>
       </c>
-      <c r="H12" s="29"/>
       <c r="I12" s="29">
         <v>-2.0</v>
       </c>
@@ -2529,45 +2556,45 @@
         <v>2.0</v>
       </c>
       <c r="K12" s="27"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="28">
+      <c r="L12" s="29">
+        <v>3.0</v>
+      </c>
+      <c r="M12" s="29">
+        <v>-1.0</v>
+      </c>
+      <c r="N12" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="O12" s="29">
         <v>1.0</v>
       </c>
-      <c r="N12" s="29">
+      <c r="P12" s="29">
+        <v>-1.0</v>
+      </c>
+      <c r="Q12" s="29">
         <v>2.0</v>
       </c>
-      <c r="O12" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="P12" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="Q12" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="R12" s="29">
-        <v>0.0</v>
-      </c>
+      <c r="R12" s="29"/>
       <c r="S12" s="29">
         <v>2.0</v>
       </c>
       <c r="T12" s="29">
-        <v>3.0</v>
-      </c>
-      <c r="U12" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="V12" s="28">
+        <v>-3.0</v>
+      </c>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29">
         <v>-1.0</v>
       </c>
       <c r="W12" s="27"/>
       <c r="X12" s="29">
         <v>2.0</v>
       </c>
-      <c r="Y12" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="Z12" s="29"/>
+      <c r="Y12" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Z12" s="29">
+        <v>2.0</v>
+      </c>
       <c r="AA12" s="29"/>
       <c r="AB12" s="29"/>
       <c r="AC12" s="30"/>
@@ -2597,15 +2624,15 @@
       </c>
       <c r="AZ12" s="5">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BA12" s="5">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BB12" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BC12" s="5">
         <f t="shared" si="4"/>
@@ -2613,15 +2640,15 @@
       </c>
       <c r="BD12" s="5">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BE12" s="5">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BF12" s="20">
         <f t="shared" si="7"/>
-        <v>0.4814814815</v>
+        <v>0.5294117647</v>
       </c>
       <c r="BG12" s="20"/>
     </row>
@@ -2634,49 +2661,49 @@
         <v>-1.0</v>
       </c>
       <c r="D13" s="29">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="E13" s="29">
         <v>0.0</v>
       </c>
       <c r="F13" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="G13" s="29">
+        <v>-3.0</v>
+      </c>
+      <c r="H13" s="29">
+        <v>3.0</v>
+      </c>
+      <c r="I13" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="J13" s="29">
         <v>2.0</v>
       </c>
-      <c r="G13" s="29">
-        <v>3.0</v>
-      </c>
-      <c r="H13" s="29">
-        <v>-3.0</v>
-      </c>
-      <c r="I13" s="29">
+      <c r="K13" s="27"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="N13" s="29">
         <v>-2.0</v>
-      </c>
-      <c r="J13" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="K13" s="27"/>
-      <c r="L13" s="29">
-        <v>-3.0</v>
-      </c>
-      <c r="M13" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="N13" s="29">
-        <v>2.0</v>
       </c>
       <c r="O13" s="29">
         <v>-1.0</v>
       </c>
-      <c r="P13" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="Q13" s="29">
-        <v>2.0</v>
-      </c>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="R13" s="29">
+        <v>0.0</v>
+      </c>
+      <c r="S13" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="T13" s="29">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="U13" s="29">
         <v>0.0</v>
@@ -2685,13 +2712,15 @@
         <v>1.0</v>
       </c>
       <c r="W13" s="27"/>
-      <c r="X13" s="28">
+      <c r="X13" s="29">
         <v>2.0</v>
       </c>
       <c r="Y13" s="29">
         <v>1.0</v>
       </c>
-      <c r="Z13" s="29"/>
+      <c r="Z13" s="29">
+        <v>2.0</v>
+      </c>
       <c r="AA13" s="29"/>
       <c r="AB13" s="29"/>
       <c r="AC13" s="30"/>
@@ -2721,7 +2750,7 @@
       </c>
       <c r="AZ13" s="5">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BA13" s="5">
         <f t="shared" si="2"/>
@@ -2729,7 +2758,7 @@
       </c>
       <c r="BB13" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BC13" s="5">
         <f t="shared" si="4"/>
@@ -2737,15 +2766,15 @@
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BE13" s="5">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="BF13" s="20">
         <f t="shared" si="7"/>
-        <v>0.4561403509</v>
+        <v>0.45</v>
       </c>
       <c r="BG13" s="20"/>
     </row>
@@ -2754,20 +2783,24 @@
         <v>68</v>
       </c>
       <c r="B14" s="27"/>
-      <c r="C14" s="29">
-        <v>-1.0</v>
+      <c r="C14" s="28">
+        <v>1.0</v>
       </c>
       <c r="D14" s="29">
+        <v>3.0</v>
+      </c>
+      <c r="E14" s="29">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29">
         <v>-3.0</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="28">
-        <v>3.0</v>
-      </c>
       <c r="I14" s="29">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="J14" s="29">
         <v>2.0</v>
@@ -2777,38 +2810,30 @@
         <v>3.0</v>
       </c>
       <c r="M14" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="N14" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="O14" s="29"/>
+      <c r="P14" s="28">
         <v>-1.0</v>
       </c>
-      <c r="N14" s="29">
+      <c r="Q14" s="29">
         <v>-2.0</v>
       </c>
-      <c r="O14" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="P14" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="Q14" s="29">
-        <v>2.0</v>
-      </c>
-      <c r="R14" s="29"/>
+      <c r="R14" s="29">
+        <v>0.0</v>
+      </c>
       <c r="S14" s="29">
         <v>2.0</v>
       </c>
-      <c r="T14" s="29">
-        <v>-3.0</v>
-      </c>
+      <c r="T14" s="29"/>
       <c r="U14" s="29"/>
-      <c r="V14" s="29">
-        <v>-1.0</v>
-      </c>
+      <c r="V14" s="29"/>
       <c r="W14" s="27"/>
-      <c r="X14" s="29">
-        <v>2.0</v>
-      </c>
-      <c r="Y14" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="X14" s="29"/>
+      <c r="Y14" s="29"/>
       <c r="Z14" s="29"/>
       <c r="AA14" s="29"/>
       <c r="AB14" s="29"/>
@@ -2839,7 +2864,7 @@
       </c>
       <c r="AZ14" s="5">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="BA14" s="5">
         <f t="shared" si="2"/>
@@ -2847,23 +2872,23 @@
       </c>
       <c r="BB14" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC14" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="BD14" s="5">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="BE14" s="5">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="BF14" s="20">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.619047619</v>
       </c>
       <c r="BG14" s="20"/>
     </row>
@@ -2878,19 +2903,15 @@
       <c r="D15" s="29">
         <v>-3.0</v>
       </c>
-      <c r="E15" s="29">
-        <v>0.0</v>
-      </c>
+      <c r="E15" s="29"/>
       <c r="F15" s="29">
         <v>-2.0</v>
       </c>
       <c r="G15" s="29">
-        <v>-3.0</v>
-      </c>
-      <c r="H15" s="29">
         <v>3.0</v>
       </c>
-      <c r="I15" s="28">
+      <c r="H15" s="29"/>
+      <c r="I15" s="29">
         <v>-2.0</v>
       </c>
       <c r="J15" s="29">
@@ -2898,24 +2919,26 @@
       </c>
       <c r="K15" s="27"/>
       <c r="L15" s="29"/>
-      <c r="M15" s="29">
+      <c r="M15" s="28">
         <v>1.0</v>
       </c>
       <c r="N15" s="29">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="O15" s="29">
         <v>-1.0</v>
       </c>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="28">
+      <c r="P15" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="Q15" s="29">
         <v>-2.0</v>
       </c>
       <c r="R15" s="29">
         <v>0.0</v>
       </c>
       <c r="S15" s="29">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="T15" s="29">
         <v>3.0</v>
@@ -2923,17 +2946,19 @@
       <c r="U15" s="29">
         <v>0.0</v>
       </c>
-      <c r="V15" s="29">
-        <v>1.0</v>
+      <c r="V15" s="28">
+        <v>-1.0</v>
       </c>
       <c r="W15" s="27"/>
       <c r="X15" s="29">
         <v>2.0</v>
       </c>
       <c r="Y15" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="Z15" s="29"/>
+        <v>-1.0</v>
+      </c>
+      <c r="Z15" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="AA15" s="29"/>
       <c r="AB15" s="29"/>
       <c r="AC15" s="30"/>
@@ -2967,11 +2992,11 @@
       </c>
       <c r="BA15" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BB15" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BC15" s="5">
         <f t="shared" si="4"/>
@@ -2979,15 +3004,15 @@
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="BE15" s="5">
         <f t="shared" si="6"/>
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="BF15" s="20">
         <f t="shared" si="7"/>
-        <v>0.4210526316</v>
+        <v>0.4561403509</v>
       </c>
       <c r="BG15" s="20"/>
     </row>
@@ -3173,7 +3198,9 @@
         <v>-2.0</v>
       </c>
       <c r="Y17" s="29"/>
-      <c r="Z17" s="29"/>
+      <c r="Z17" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="AA17" s="29"/>
       <c r="AB17" s="29"/>
       <c r="AC17" s="30"/>
@@ -3203,7 +3230,7 @@
       </c>
       <c r="AZ17" s="5">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BA17" s="5">
         <f t="shared" si="2"/>
@@ -3215,7 +3242,7 @@
       </c>
       <c r="BC17" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="5"/>
@@ -3223,11 +3250,11 @@
       </c>
       <c r="BE17" s="5">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF17" s="20">
         <f t="shared" si="7"/>
-        <v>0.5111111111</v>
+        <v>0.4791666667</v>
       </c>
       <c r="BG17" s="20"/>
     </row>
@@ -3293,7 +3320,9 @@
       <c r="Y18" s="29">
         <v>1.0</v>
       </c>
-      <c r="Z18" s="29"/>
+      <c r="Z18" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="AA18" s="29"/>
       <c r="AB18" s="29"/>
       <c r="AC18" s="30"/>
@@ -3323,7 +3352,7 @@
       </c>
       <c r="AZ18" s="5">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BA18" s="5">
         <f t="shared" si="2"/>
@@ -3335,7 +3364,7 @@
       </c>
       <c r="BC18" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD18" s="5">
         <f t="shared" si="5"/>
@@ -3343,11 +3372,11 @@
       </c>
       <c r="BE18" s="5">
         <f t="shared" si="6"/>
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="BF18" s="20">
         <f t="shared" si="7"/>
-        <v>0.4509803922</v>
+        <v>0.4259259259</v>
       </c>
       <c r="BG18" s="20"/>
     </row>
@@ -3411,7 +3440,9 @@
       <c r="W19" s="27"/>
       <c r="X19" s="29"/>
       <c r="Y19" s="29"/>
-      <c r="Z19" s="29"/>
+      <c r="Z19" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="AA19" s="29"/>
       <c r="AB19" s="29"/>
       <c r="AC19" s="30"/>
@@ -3441,7 +3472,7 @@
       </c>
       <c r="AZ19" s="5">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BA19" s="5">
         <f t="shared" si="2"/>
@@ -3453,7 +3484,7 @@
       </c>
       <c r="BC19" s="5">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BD19" s="5">
         <f t="shared" si="5"/>
@@ -3461,11 +3492,11 @@
       </c>
       <c r="BE19" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="BF19" s="20">
         <f t="shared" si="7"/>
-        <v>0.4375</v>
+        <v>0.4117647059</v>
       </c>
       <c r="BG19" s="20"/>
     </row>
@@ -3477,50 +3508,42 @@
       <c r="C20" s="29">
         <v>1.0</v>
       </c>
-      <c r="D20" s="28">
-        <v>3.0</v>
+      <c r="D20" s="29">
+        <v>-3.0</v>
       </c>
       <c r="E20" s="29">
         <v>0.0</v>
       </c>
-      <c r="F20" s="29">
-        <v>-2.0</v>
-      </c>
+      <c r="F20" s="29"/>
       <c r="G20" s="29">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="H20" s="29">
         <v>-3.0</v>
       </c>
-      <c r="I20" s="29">
+      <c r="I20" s="28">
         <v>2.0</v>
       </c>
       <c r="J20" s="29">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="29">
         <v>-3.0</v>
       </c>
-      <c r="M20" s="28">
+      <c r="M20" s="29">
         <v>-1.0</v>
       </c>
-      <c r="N20" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="O20" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="P20" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="Q20" s="29">
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="28">
         <v>2.0</v>
       </c>
-      <c r="R20" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="S20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29">
+        <v>2.0</v>
+      </c>
       <c r="T20" s="29">
         <v>-3.0</v>
       </c>
@@ -3534,8 +3557,12 @@
       <c r="X20" s="29">
         <v>-2.0</v>
       </c>
-      <c r="Y20" s="29"/>
-      <c r="Z20" s="29"/>
+      <c r="Y20" s="29">
+        <v>-1.0</v>
+      </c>
+      <c r="Z20" s="29">
+        <v>2.0</v>
+      </c>
       <c r="AA20" s="29"/>
       <c r="AB20" s="29"/>
       <c r="AC20" s="30"/>
@@ -3565,31 +3592,31 @@
       </c>
       <c r="AZ20" s="5">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="BA20" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB20" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BC20" s="5">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="6"/>
-        <v>-12</v>
+        <v>-7</v>
       </c>
       <c r="BF20" s="20">
         <f t="shared" si="7"/>
-        <v>0.3157894737</v>
+        <v>0.3921568627</v>
       </c>
       <c r="BG20" s="20"/>
     </row>
@@ -3601,42 +3628,50 @@
       <c r="C21" s="29">
         <v>1.0</v>
       </c>
-      <c r="D21" s="29">
-        <v>-3.0</v>
+      <c r="D21" s="28">
+        <v>3.0</v>
       </c>
       <c r="E21" s="29">
         <v>0.0</v>
       </c>
-      <c r="F21" s="29"/>
+      <c r="F21" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="G21" s="29">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="H21" s="29">
         <v>-3.0</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="29">
         <v>2.0</v>
       </c>
       <c r="J21" s="29">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="29">
         <v>-3.0</v>
       </c>
-      <c r="M21" s="29">
+      <c r="M21" s="28">
         <v>-1.0</v>
       </c>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="28">
+      <c r="N21" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="O21" s="29">
+        <v>-1.0</v>
+      </c>
+      <c r="P21" s="29">
+        <v>-1.0</v>
+      </c>
+      <c r="Q21" s="29">
         <v>2.0</v>
       </c>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29">
-        <v>2.0</v>
-      </c>
+      <c r="R21" s="29">
+        <v>0.0</v>
+      </c>
+      <c r="S21" s="29"/>
       <c r="T21" s="29">
         <v>-3.0</v>
       </c>
@@ -3650,10 +3685,10 @@
       <c r="X21" s="29">
         <v>-2.0</v>
       </c>
-      <c r="Y21" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="Z21" s="29"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="AA21" s="29"/>
       <c r="AB21" s="29"/>
       <c r="AC21" s="30"/>
@@ -3683,7 +3718,7 @@
       </c>
       <c r="AZ21" s="5">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="BA21" s="5">
         <f t="shared" si="2"/>
@@ -3691,23 +3726,23 @@
       </c>
       <c r="BB21" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BC21" s="5">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BD21" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BE21" s="5">
         <f t="shared" si="6"/>
-        <v>-9</v>
+        <v>-14</v>
       </c>
       <c r="BF21" s="20">
         <f t="shared" si="7"/>
-        <v>0.3541666667</v>
+        <v>0.3</v>
       </c>
       <c r="BG21" s="20"/>
     </row>
@@ -4018,52 +4053,40 @@
       <c r="B25" s="27"/>
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
-      <c r="E25" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="F25" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
       <c r="G25" s="29"/>
-      <c r="H25" s="29">
-        <v>3.0</v>
-      </c>
+      <c r="H25" s="29"/>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
       <c r="K25" s="27"/>
       <c r="L25" s="29"/>
-      <c r="M25" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="N25" s="29">
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="P25" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="Q25" s="29">
         <v>-2.0</v>
       </c>
-      <c r="O25" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="28">
-        <v>0.0</v>
-      </c>
+      <c r="R25" s="29"/>
       <c r="S25" s="29">
         <v>-2.0</v>
       </c>
-      <c r="T25" s="29">
-        <v>-3.0</v>
-      </c>
-      <c r="U25" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="V25" s="29">
+      <c r="T25" s="29"/>
+      <c r="U25" s="29"/>
+      <c r="V25" s="29"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="29"/>
+      <c r="Y25" s="29">
         <v>-1.0</v>
       </c>
-      <c r="W25" s="27"/>
-      <c r="X25" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="Y25" s="29"/>
-      <c r="Z25" s="29"/>
+      <c r="Z25" s="28">
+        <v>2.0</v>
+      </c>
       <c r="AA25" s="29"/>
       <c r="AB25" s="29"/>
       <c r="AC25" s="30"/>
@@ -4093,19 +4116,19 @@
       </c>
       <c r="AZ25" s="5">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="BA25" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB25" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC25" s="5">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BD25" s="5">
         <f t="shared" si="5"/>
@@ -4113,11 +4136,11 @@
       </c>
       <c r="BE25" s="5">
         <f t="shared" si="6"/>
-        <v>-7</v>
+        <v>-1</v>
       </c>
       <c r="BF25" s="20">
         <f t="shared" si="7"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="BG25" s="20"/>
     </row>
@@ -4126,38 +4149,52 @@
         <v>80</v>
       </c>
       <c r="B26" s="27"/>
-      <c r="C26" s="29">
-        <v>-1.0</v>
-      </c>
+      <c r="C26" s="29"/>
       <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29">
-        <v>-3.0</v>
-      </c>
-      <c r="H26" s="29"/>
+      <c r="E26" s="29">
+        <v>0.0</v>
+      </c>
+      <c r="F26" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29">
+        <v>3.0</v>
+      </c>
       <c r="I26" s="29"/>
       <c r="J26" s="29"/>
       <c r="K26" s="27"/>
-      <c r="L26" s="28">
-        <v>3.0</v>
-      </c>
+      <c r="L26" s="29"/>
       <c r="M26" s="29">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="N26" s="29">
         <v>-2.0</v>
       </c>
-      <c r="O26" s="29"/>
+      <c r="O26" s="29">
+        <v>-1.0</v>
+      </c>
       <c r="P26" s="29"/>
       <c r="Q26" s="29"/>
-      <c r="R26" s="29"/>
-      <c r="S26" s="29"/>
-      <c r="T26" s="29"/>
-      <c r="U26" s="29"/>
-      <c r="V26" s="29"/>
+      <c r="R26" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="S26" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="T26" s="29">
+        <v>-3.0</v>
+      </c>
+      <c r="U26" s="29">
+        <v>0.0</v>
+      </c>
+      <c r="V26" s="29">
+        <v>-1.0</v>
+      </c>
       <c r="W26" s="27"/>
-      <c r="X26" s="29"/>
+      <c r="X26" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="Y26" s="29"/>
       <c r="Z26" s="29"/>
       <c r="AA26" s="29"/>
@@ -4189,7 +4226,7 @@
       </c>
       <c r="AZ26" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="BA26" s="5">
         <f t="shared" si="2"/>
@@ -4197,23 +4234,23 @@
       </c>
       <c r="BB26" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BC26" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BD26" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BE26" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-7</v>
       </c>
       <c r="BF26" s="20">
         <f t="shared" si="7"/>
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="BG26" s="20"/>
     </row>
@@ -4237,16 +4274,14 @@
       <c r="O27" s="29">
         <v>1.0</v>
       </c>
-      <c r="P27" s="29">
-        <v>1.0</v>
-      </c>
+      <c r="P27" s="29"/>
       <c r="Q27" s="29">
         <v>-2.0</v>
       </c>
-      <c r="R27" s="29"/>
-      <c r="S27" s="29">
-        <v>-2.0</v>
-      </c>
+      <c r="R27" s="29">
+        <v>0.0</v>
+      </c>
+      <c r="S27" s="29"/>
       <c r="T27" s="29"/>
       <c r="U27" s="29"/>
       <c r="V27" s="29"/>
@@ -4255,7 +4290,9 @@
       <c r="Y27" s="29">
         <v>-1.0</v>
       </c>
-      <c r="Z27" s="29"/>
+      <c r="Z27" s="29">
+        <v>2.0</v>
+      </c>
       <c r="AA27" s="29"/>
       <c r="AB27" s="29"/>
       <c r="AC27" s="30"/>
@@ -4293,23 +4330,23 @@
       </c>
       <c r="BB27" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC27" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BD27" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE27" s="5">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="BF27" s="20">
         <f t="shared" si="7"/>
-        <v>0.4</v>
+        <v>0.4666666667</v>
       </c>
       <c r="BG27" s="20"/>
     </row>
@@ -4318,38 +4355,34 @@
         <v>82</v>
       </c>
       <c r="B28" s="27"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29">
+      <c r="C28" s="29">
+        <v>-1.0</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29">
         <v>-3.0</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="G28" s="29"/>
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
       <c r="J28" s="29"/>
       <c r="K28" s="27"/>
-      <c r="L28" s="29">
-        <v>-3.0</v>
-      </c>
-      <c r="M28" s="29"/>
-      <c r="N28" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="O28" s="29">
-        <v>-1.0</v>
-      </c>
-      <c r="P28" s="29">
-        <v>-1.0</v>
-      </c>
+      <c r="L28" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="M28" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="N28" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
       <c r="Q28" s="29"/>
       <c r="R28" s="29"/>
       <c r="S28" s="29"/>
-      <c r="T28" s="29">
-        <v>3.0</v>
-      </c>
+      <c r="T28" s="29"/>
       <c r="U28" s="29"/>
       <c r="V28" s="29"/>
       <c r="W28" s="27"/>
@@ -4385,7 +4418,7 @@
       </c>
       <c r="AZ28" s="5">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="BA28" s="5">
         <f t="shared" si="2"/>
@@ -4397,7 +4430,7 @@
       </c>
       <c r="BC28" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BD28" s="5">
         <f t="shared" si="5"/>
@@ -4405,11 +4438,11 @@
       </c>
       <c r="BE28" s="5">
         <f t="shared" si="6"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="BF28" s="20">
         <f t="shared" si="7"/>
-        <v>0.2857142857</v>
+        <v>0.4</v>
       </c>
       <c r="BG28" s="20"/>
     </row>
@@ -4419,23 +4452,37 @@
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
+      <c r="D29" s="29">
+        <v>-3.0</v>
+      </c>
       <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+      <c r="F29" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
       <c r="J29" s="29"/>
       <c r="K29" s="27"/>
-      <c r="L29" s="29"/>
+      <c r="L29" s="29">
+        <v>-3.0</v>
+      </c>
       <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="29"/>
-      <c r="P29" s="29"/>
+      <c r="N29" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="O29" s="29">
+        <v>-1.0</v>
+      </c>
+      <c r="P29" s="29">
+        <v>-1.0</v>
+      </c>
       <c r="Q29" s="29"/>
       <c r="R29" s="29"/>
       <c r="S29" s="29"/>
-      <c r="T29" s="29"/>
+      <c r="T29" s="29">
+        <v>3.0</v>
+      </c>
       <c r="U29" s="29"/>
       <c r="V29" s="29"/>
       <c r="W29" s="27"/>
@@ -4466,16 +4513,16 @@
       <c r="AV29" s="29"/>
       <c r="AW29" s="29"/>
       <c r="AX29" s="29"/>
-      <c r="AY29" s="37">
+      <c r="AY29" s="19">
         <v>25.0</v>
       </c>
       <c r="AZ29" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BA29" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB29" s="5">
         <f t="shared" si="3"/>
@@ -4483,19 +4530,19 @@
       </c>
       <c r="BC29" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BD29" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BE29" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BF29" s="20" t="str">
+        <v>-5</v>
+      </c>
+      <c r="BF29" s="20">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>0.2857142857</v>
       </c>
       <c r="BG29" s="20"/>
     </row>
@@ -4552,7 +4599,7 @@
       <c r="AV30" s="29"/>
       <c r="AW30" s="29"/>
       <c r="AX30" s="29"/>
-      <c r="AY30" s="37">
+      <c r="AY30" s="19">
         <v>26.0</v>
       </c>
       <c r="AZ30" s="5">
@@ -4592,9 +4639,7 @@
       <c r="B31" s="27"/>
       <c r="C31" s="29"/>
       <c r="D31" s="29"/>
-      <c r="E31" s="29">
-        <v>0.0</v>
-      </c>
+      <c r="E31" s="29"/>
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
       <c r="H31" s="29"/>
@@ -4614,9 +4659,7 @@
       <c r="V31" s="29"/>
       <c r="W31" s="27"/>
       <c r="X31" s="29"/>
-      <c r="Y31" s="29">
-        <v>1.0</v>
-      </c>
+      <c r="Y31" s="29"/>
       <c r="Z31" s="29"/>
       <c r="AA31" s="29"/>
       <c r="AB31" s="29"/>
@@ -4642,20 +4685,20 @@
       <c r="AV31" s="29"/>
       <c r="AW31" s="29"/>
       <c r="AX31" s="29"/>
-      <c r="AY31" s="37">
+      <c r="AY31" s="19">
         <v>27.0</v>
       </c>
       <c r="AZ31" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BA31" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB31" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC31" s="5">
         <f t="shared" si="4"/>
@@ -4663,19 +4706,19 @@
       </c>
       <c r="BD31" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BE31" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="BF31" s="20">
+        <v>0</v>
+      </c>
+      <c r="BF31" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0.6666666667</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="BG31" s="20"/>
     </row>
-    <row r="32" ht="13.5" customHeight="1">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="36" t="s">
         <v>86</v>
       </c>
@@ -4728,8 +4771,8 @@
       <c r="AV32" s="29"/>
       <c r="AW32" s="29"/>
       <c r="AX32" s="29"/>
-      <c r="AY32" s="37">
-        <v>28.0</v>
+      <c r="AY32" s="19">
+        <v>29.0</v>
       </c>
       <c r="AZ32" s="5">
         <f t="shared" si="1"/>
@@ -4778,25 +4821,17 @@
       <c r="L33" s="29"/>
       <c r="M33" s="29"/>
       <c r="N33" s="29"/>
-      <c r="O33" s="29">
-        <v>1.0</v>
-      </c>
+      <c r="O33" s="29"/>
       <c r="P33" s="29"/>
-      <c r="Q33" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="R33" s="29">
-        <v>0.0</v>
-      </c>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
       <c r="S33" s="29"/>
       <c r="T33" s="29"/>
       <c r="U33" s="29"/>
       <c r="V33" s="29"/>
       <c r="W33" s="27"/>
       <c r="X33" s="29"/>
-      <c r="Y33" s="29">
-        <v>-1.0</v>
-      </c>
+      <c r="Y33" s="29"/>
       <c r="Z33" s="29"/>
       <c r="AA33" s="29"/>
       <c r="AB33" s="29"/>
@@ -4822,36 +4857,36 @@
       <c r="AV33" s="29"/>
       <c r="AW33" s="29"/>
       <c r="AX33" s="29"/>
-      <c r="AY33" s="37">
-        <v>29.0</v>
+      <c r="AY33" s="19">
+        <v>30.0</v>
       </c>
       <c r="AZ33" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BA33" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB33" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC33" s="5">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BD33" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BE33" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
-      </c>
-      <c r="BF33" s="20">
+        <v>0</v>
+      </c>
+      <c r="BF33" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0.3333333333</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="BG33" s="20"/>
     </row>
@@ -4862,7 +4897,9 @@
       <c r="B34" s="27"/>
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
+      <c r="E34" s="29">
+        <v>0.0</v>
+      </c>
       <c r="F34" s="29"/>
       <c r="G34" s="29"/>
       <c r="H34" s="29"/>
@@ -4882,7 +4919,9 @@
       <c r="V34" s="29"/>
       <c r="W34" s="27"/>
       <c r="X34" s="29"/>
-      <c r="Y34" s="29"/>
+      <c r="Y34" s="29">
+        <v>1.0</v>
+      </c>
       <c r="Z34" s="29"/>
       <c r="AA34" s="29"/>
       <c r="AB34" s="29"/>
@@ -4908,20 +4947,20 @@
       <c r="AV34" s="29"/>
       <c r="AW34" s="29"/>
       <c r="AX34" s="29"/>
-      <c r="AY34" s="37">
-        <v>30.0</v>
+      <c r="AY34" s="19">
+        <v>28.0</v>
       </c>
       <c r="AZ34" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA34" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB34" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC34" s="5">
         <f t="shared" si="4"/>
@@ -4929,19 +4968,19 @@
       </c>
       <c r="BD34" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BE34" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BF34" s="20" t="str">
+        <v>1</v>
+      </c>
+      <c r="BF34" s="20">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>0.6666666667</v>
       </c>
       <c r="BG34" s="20"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="36" t="s">
         <v>89</v>
       </c>
@@ -4994,8 +5033,8 @@
       <c r="AV35" s="29"/>
       <c r="AW35" s="29"/>
       <c r="AX35" s="29"/>
-      <c r="AY35" s="37">
-        <v>31.0</v>
+      <c r="AY35" s="19">
+        <v>32.0</v>
       </c>
       <c r="AZ35" s="5">
         <f t="shared" si="1"/>
@@ -5090,8 +5129,8 @@
       <c r="AV36" s="29"/>
       <c r="AW36" s="29"/>
       <c r="AX36" s="29"/>
-      <c r="AY36" s="37">
-        <v>32.0</v>
+      <c r="AY36" s="19">
+        <v>31.0</v>
       </c>
       <c r="AZ36" s="5">
         <f t="shared" si="1"/>
@@ -5392,7 +5431,7 @@
       <c r="BG39" s="20"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="37" t="s">
         <v>94</v>
       </c>
       <c r="B40" s="27"/>
@@ -5401,12 +5440,8 @@
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>
-      <c r="H40" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="I40" s="29">
-        <v>-2.0</v>
-      </c>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
       <c r="J40" s="29"/>
       <c r="K40" s="27"/>
       <c r="L40" s="29"/>
@@ -5453,7 +5488,7 @@
       </c>
       <c r="AZ40" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BA40" s="5">
         <f t="shared" si="2"/>
@@ -5461,23 +5496,23 @@
       </c>
       <c r="BB40" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC40" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD40" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE40" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
-      </c>
-      <c r="BF40" s="20">
+        <v>0</v>
+      </c>
+      <c r="BF40" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0.1666666667</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="BG40" s="20"/>
     </row>
@@ -5511,11 +5546,11 @@
       </c>
       <c r="H41" s="33">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I41" s="33">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J41" s="33">
         <f t="shared" si="8"/>
@@ -5583,7 +5618,7 @@
       </c>
       <c r="Z41" s="33">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AA41" s="33">
         <f t="shared" si="8"/>
@@ -5757,7 +5792,9 @@
       <c r="Y42" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="Z42" s="41"/>
+      <c r="Z42" s="41" t="s">
+        <v>111</v>
+      </c>
       <c r="AA42" s="41"/>
       <c r="AB42" s="41"/>
       <c r="AC42" s="5"/>
@@ -5791,7 +5828,7 @@
       <c r="BF42" s="20"/>
       <c r="BG42" s="20"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43">
       <c r="A43" s="2"/>
       <c r="B43" s="5"/>
       <c r="C43" s="42"/>
@@ -26049,28 +26086,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G1" s="44" t="s">
         <v>56</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
@@ -26093,13 +26130,13 @@
         <v>3.0</v>
       </c>
       <c r="G3" s="45">
-        <f t="shared" ref="G3:G36" si="1">SUM(C3*3)+D3</f>
+        <f t="shared" ref="G3:G26" si="1">SUM(C3*3)+D3</f>
         <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="44">
         <v>2.0</v>
@@ -26130,7 +26167,7 @@
     </row>
     <row r="5">
       <c r="A5" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" s="44">
         <v>2.0</v>
@@ -26161,7 +26198,7 @@
     </row>
     <row r="6">
       <c r="A6" s="26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B6" s="44">
         <v>2.0</v>
@@ -26192,7 +26229,7 @@
     </row>
     <row r="7">
       <c r="A7" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B7" s="45">
         <v>2.0</v>
@@ -26223,7 +26260,7 @@
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B8" s="44">
         <v>1.0</v>
@@ -26279,7 +26316,7 @@
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B10" s="44">
         <v>1.0</v>
@@ -26304,10 +26341,10 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="B11" s="44">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C11" s="44">
         <v>1.0</v>
@@ -26316,7 +26353,7 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="44">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F11" s="44">
         <v>2.0</v>
@@ -26330,7 +26367,7 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B12" s="44">
         <v>2.0</v>
@@ -26345,7 +26382,7 @@
         <v>1.0</v>
       </c>
       <c r="F12" s="44">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G12" s="44">
         <f t="shared" si="1"/>
@@ -26355,7 +26392,7 @@
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B13" s="44">
         <v>2.0</v>
@@ -26380,13 +26417,13 @@
         <v>25.0</v>
       </c>
       <c r="J13" s="46">
-        <f t="shared" ref="J13:J27" si="3">I13/B13</f>
+        <f t="shared" ref="J13:J25" si="3">I13/B13</f>
         <v>12.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B14" s="44">
         <v>2.0</v>
@@ -26418,7 +26455,7 @@
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="B15" s="44">
         <v>2.0</v>
@@ -26449,7 +26486,7 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
       <c r="B16" s="44">
         <v>2.0</v>
@@ -26480,7 +26517,7 @@
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B17" s="44">
         <v>2.0</v>
@@ -26495,7 +26532,7 @@
         <v>1.0</v>
       </c>
       <c r="F17" s="44">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G17" s="44">
         <f t="shared" si="1"/>
@@ -26511,26 +26548,26 @@
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B18" s="44">
         <v>2.0</v>
       </c>
       <c r="C18" s="44">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="44">
         <v>0.0</v>
       </c>
-      <c r="D18" s="44">
-        <v>2.0</v>
-      </c>
       <c r="E18" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F18" s="44">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G18" s="44">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I18" s="47">
         <v>19.0</v>
@@ -26542,7 +26579,7 @@
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B19" s="44">
         <v>2.0</v>
@@ -26551,17 +26588,17 @@
         <v>0.0</v>
       </c>
       <c r="D19" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E19" s="44">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F19" s="44">
-        <v>-2.0</v>
+        <v>0.0</v>
       </c>
       <c r="G19" s="44">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19" s="47">
         <v>15.0</v>
@@ -26573,7 +26610,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B20" s="44">
         <v>2.0</v>
@@ -26588,7 +26625,7 @@
         <v>1.0</v>
       </c>
       <c r="F20" s="44">
-        <v>-3.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G20" s="44">
         <f t="shared" si="1"/>
@@ -26604,16 +26641,16 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B21" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C21" s="44">
         <v>0.0</v>
       </c>
       <c r="D21" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E21" s="44">
         <v>1.0</v>
@@ -26623,19 +26660,19 @@
       </c>
       <c r="G21" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="47">
         <v>25.0</v>
       </c>
       <c r="J21" s="46">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B22" s="44">
         <v>1.0</v>
@@ -26666,10 +26703,10 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B23" s="44">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C23" s="44">
         <v>0.0</v>
@@ -26678,10 +26715,10 @@
         <v>0.0</v>
       </c>
       <c r="E23" s="44">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F23" s="44">
-        <v>-4.0</v>
+        <v>-3.0</v>
       </c>
       <c r="G23" s="44">
         <f t="shared" si="1"/>
@@ -26692,12 +26729,12 @@
       </c>
       <c r="J23" s="46">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B24" s="44">
         <v>2.0</v>
@@ -26728,7 +26765,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B25" s="44">
         <v>2.0</v>
@@ -26759,132 +26796,38 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>93</v>
+        <v>64</v>
+      </c>
+      <c r="B26" s="44">
+        <v>3.0</v>
+      </c>
+      <c r="C26" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="E26" s="44">
+        <v>3.0</v>
+      </c>
+      <c r="F26" s="44">
+        <v>-6.0</v>
       </c>
       <c r="G26" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I26" s="47">
-        <v>8.0</v>
-      </c>
-      <c r="J26" s="46" t="str">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="47">
-        <v>1.0</v>
-      </c>
-      <c r="J27" s="46" t="str">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="G28" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="47">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="G29" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="47">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="47">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="G31" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="44">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="G32" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="44">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G33" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="G34" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
+    </row>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
@@ -28168,7 +28111,7 @@
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="29">
@@ -28244,7 +28187,7 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29">
@@ -28322,7 +28265,7 @@
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="29">
@@ -28400,7 +28343,7 @@
     </row>
     <row r="6">
       <c r="A6" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="29">
@@ -28478,7 +28421,7 @@
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
@@ -28548,7 +28491,7 @@
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="29"/>
@@ -28700,7 +28643,7 @@
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="29"/>
@@ -28772,7 +28715,7 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="27"/>
       <c r="C11" s="29"/>
@@ -28917,7 +28860,7 @@
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="29"/>
@@ -28991,7 +28934,7 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="29"/>
@@ -29067,7 +29010,7 @@
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="29"/>
@@ -29354,7 +29297,7 @@
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B19" s="27"/>
       <c r="C19" s="29"/>
@@ -29634,7 +29577,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="29"/>
@@ -29702,7 +29645,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="29"/>
@@ -29770,7 +29713,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="29"/>
@@ -30098,7 +30041,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B30" s="27"/>
       <c r="C30" s="29"/>
@@ -30160,7 +30103,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="29"/>
@@ -30346,7 +30289,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="36" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B34" s="27"/>
       <c r="C34" s="29"/>
@@ -30408,7 +30351,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B35" s="27"/>
       <c r="C35" s="29"/>
@@ -30470,7 +30413,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="36" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="B36" s="27"/>
       <c r="C36" s="29"/>
@@ -30495,7 +30438,9 @@
       <c r="V36" s="29"/>
       <c r="W36" s="27"/>
       <c r="X36" s="29"/>
-      <c r="Y36" s="29"/>
+      <c r="Y36" s="29">
+        <v>1.0</v>
+      </c>
       <c r="Z36" s="29"/>
       <c r="AA36" s="29"/>
       <c r="AB36" s="29"/>
@@ -30525,7 +30470,7 @@
       <c r="AZ36" s="6"/>
       <c r="BA36" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB36" s="5"/>
       <c r="BC36" s="5"/>
@@ -30649,11 +30594,11 @@
       </c>
       <c r="H39" s="44">
         <f>'League Table'!H41</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I39" s="44">
         <f>'League Table'!I41</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J39" s="44">
         <f>'League Table'!J41</f>
@@ -30721,7 +30666,7 @@
       </c>
       <c r="Z39" s="44">
         <f>'League Table'!Z41</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AA39" s="44">
         <f>'League Table'!AA41</f>
@@ -30853,7 +30798,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="44" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B41" s="44">
         <f t="shared" ref="B41:AV41" si="2">SUM(B3:B37)</f>
@@ -30949,7 +30894,7 @@
       </c>
       <c r="Y41" s="44">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z41" s="44">
         <f t="shared" si="2"/>
@@ -61771,7 +61716,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="2"/>
@@ -61939,7 +61884,7 @@
         <v>121</v>
       </c>
       <c r="BA3" s="53" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
@@ -61998,7 +61943,7 @@
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16">
@@ -62048,7 +61993,9 @@
       <c r="Y5" s="16">
         <v>1.0</v>
       </c>
-      <c r="Z5" s="16"/>
+      <c r="Z5" s="16">
+        <v>1.0</v>
+      </c>
       <c r="AA5" s="16"/>
       <c r="AB5" s="16"/>
       <c r="AC5" s="16"/>
@@ -62076,7 +62023,7 @@
       <c r="AY5" s="16"/>
       <c r="BA5" s="44">
         <f t="shared" ref="BA5:BA37" si="1">SUM(B5:AY5)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -62129,7 +62076,9 @@
       <c r="Y6" s="33">
         <v>2.0</v>
       </c>
-      <c r="Z6" s="33"/>
+      <c r="Z6" s="33">
+        <v>2.0</v>
+      </c>
       <c r="AA6" s="33"/>
       <c r="AB6" s="33"/>
       <c r="AC6" s="33"/>
@@ -62157,12 +62106,12 @@
       <c r="AY6" s="33"/>
       <c r="BA6" s="44">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="29">
@@ -62237,7 +62186,7 @@
     </row>
     <row r="8">
       <c r="A8" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16">
@@ -62312,7 +62261,7 @@
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
@@ -62383,7 +62332,7 @@
     </row>
     <row r="10">
       <c r="A10" s="31" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
@@ -62419,7 +62368,9 @@
       <c r="W10" s="27"/>
       <c r="X10" s="29"/>
       <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
+      <c r="Z10" s="29">
+        <v>1.0</v>
+      </c>
       <c r="AA10" s="29"/>
       <c r="AB10" s="29"/>
       <c r="AC10" s="29"/>
@@ -62447,12 +62398,12 @@
       <c r="AY10" s="29"/>
       <c r="BA10" s="44">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
@@ -62488,7 +62439,9 @@
       <c r="Y11" s="29">
         <v>1.0</v>
       </c>
-      <c r="Z11" s="29"/>
+      <c r="Z11" s="29">
+        <v>2.0</v>
+      </c>
       <c r="AA11" s="29"/>
       <c r="AB11" s="29"/>
       <c r="AC11" s="29"/>
@@ -62516,36 +62469,36 @@
       <c r="AY11" s="29"/>
       <c r="BA11" s="44">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="33"/>
-      <c r="D12" s="33">
+      <c r="D12" s="33"/>
+      <c r="E12" s="33">
         <v>1.0</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
+      <c r="F12" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>1.0</v>
+      </c>
       <c r="H12" s="33"/>
       <c r="I12" s="33"/>
       <c r="J12" s="33"/>
       <c r="K12" s="33"/>
       <c r="L12" s="33"/>
       <c r="M12" s="33"/>
-      <c r="N12" s="33">
-        <v>1.0</v>
-      </c>
+      <c r="N12" s="33"/>
       <c r="O12" s="33">
         <v>1.0</v>
       </c>
-      <c r="P12" s="33">
-        <v>1.0</v>
-      </c>
+      <c r="P12" s="33"/>
       <c r="Q12" s="33"/>
       <c r="R12" s="33"/>
       <c r="S12" s="33"/>
@@ -62555,7 +62508,9 @@
       <c r="W12" s="32"/>
       <c r="X12" s="33"/>
       <c r="Y12" s="33"/>
-      <c r="Z12" s="33"/>
+      <c r="Z12" s="33">
+        <v>1.0</v>
+      </c>
       <c r="AA12" s="33"/>
       <c r="AB12" s="33"/>
       <c r="AC12" s="33"/>
@@ -62583,36 +62538,36 @@
       <c r="AY12" s="33"/>
       <c r="BA12" s="44">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29">
+      <c r="D13" s="29">
         <v>1.0</v>
       </c>
-      <c r="F13" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="G13" s="29">
-        <v>1.0</v>
-      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
       <c r="K13" s="29"/>
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
+      <c r="N13" s="29">
+        <v>1.0</v>
+      </c>
       <c r="O13" s="29">
         <v>1.0</v>
       </c>
-      <c r="P13" s="29"/>
+      <c r="P13" s="29">
+        <v>1.0</v>
+      </c>
       <c r="Q13" s="29"/>
       <c r="R13" s="29"/>
       <c r="S13" s="29"/>
@@ -62655,7 +62610,7 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
@@ -62781,7 +62736,7 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -62903,7 +62858,7 @@
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -62964,7 +62919,7 @@
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -63086,16 +63041,14 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="29">
-        <v>1.0</v>
-      </c>
+      <c r="G21" s="29"/>
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
@@ -63114,7 +63067,9 @@
       <c r="W21" s="27"/>
       <c r="X21" s="29"/>
       <c r="Y21" s="29"/>
-      <c r="Z21" s="29"/>
+      <c r="Z21" s="29">
+        <v>1.0</v>
+      </c>
       <c r="AA21" s="29"/>
       <c r="AB21" s="29"/>
       <c r="AC21" s="29"/>
@@ -63147,14 +63102,16 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
       <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
+      <c r="G22" s="29">
+        <v>1.0</v>
+      </c>
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
       <c r="J22" s="29"/>
@@ -63201,12 +63158,12 @@
       <c r="AY22" s="29"/>
       <c r="BA22" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -63265,7 +63222,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -63324,7 +63281,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -63383,7 +63340,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
@@ -63442,7 +63399,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
@@ -63501,7 +63458,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="36" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
@@ -63619,7 +63576,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
@@ -63678,7 +63635,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
@@ -63737,7 +63694,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
@@ -63796,7 +63753,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
@@ -64032,7 +63989,7 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
@@ -64250,7 +64207,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B41" s="5">
         <f t="shared" ref="B41:AY41" si="2">SUM(B5:B39)</f>
@@ -64350,7 +64307,7 @@
       </c>
       <c r="Z41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA41" s="5">
         <f t="shared" si="2"/>
@@ -64454,7 +64411,7 @@
       </c>
       <c r="BA41" s="44">
         <f>SUM(B41:AZ41)</f>
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -65441,19 +65398,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="44" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -65469,16 +65426,16 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="5"/>
@@ -65490,10 +65447,10 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="49"/>
@@ -65507,16 +65464,16 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="5"/>
@@ -65528,16 +65485,16 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="5"/>
@@ -65549,27 +65506,27 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="G7" s="49"/>
       <c r="H7" s="5" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="I7" s="5"/>
       <c r="K7" s="44" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="M7" s="44" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="N7" s="5"/>
     </row>
@@ -65578,16 +65535,16 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G8" s="49"/>
       <c r="H8" s="5"/>
@@ -65599,35 +65556,35 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G9" s="49"/>
       <c r="H9" s="5" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="I9" s="5">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="L9" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="N9" s="5">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="10">
@@ -65635,35 +65592,35 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E10" s="49" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="5" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="I10" s="5">
         <v>4.0</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="L10" s="5">
         <v>2.0</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="N10" s="5">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="11">
@@ -65671,32 +65628,32 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G11" s="49"/>
       <c r="H11" s="5" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="I11" s="5">
         <v>3.0</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="L11" s="5">
         <v>2.0</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N11" s="5">
         <v>4.0</v>
@@ -65707,30 +65664,30 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I12" s="5">
         <v>3.0</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="N12" s="5">
         <v>4.0</v>
@@ -65741,31 +65698,31 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F13" s="49"/>
       <c r="G13" s="49"/>
       <c r="H13" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="I13" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="N13" s="5">
         <v>4.0</v>
@@ -65776,33 +65733,33 @@
         <v>12.0</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G14" s="49"/>
       <c r="H14" s="5" t="s">
-        <v>148</v>
+        <v>179</v>
       </c>
       <c r="I14" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="N14" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="15">
@@ -65810,30 +65767,30 @@
         <v>13.0</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="5" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="I15" s="5">
         <v>2.0</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="N15" s="5">
         <v>3.0</v>
@@ -65844,30 +65801,30 @@
         <v>14.0</v>
       </c>
       <c r="B16" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="C16" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="D16" s="49" t="s">
-        <v>175</v>
-      </c>
       <c r="E16" s="49" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I16" s="5">
         <v>2.0</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="N16" s="5">
         <v>3.0</v>
@@ -65878,30 +65835,30 @@
         <v>15.0</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="5" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="I17" s="5">
         <v>2.0</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N17" s="5">
         <v>3.0</v>
@@ -65912,33 +65869,33 @@
         <v>16.0</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="I18" s="5">
         <v>2.0</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="N18" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="19">
@@ -65946,28 +65903,30 @@
         <v>17.0</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E19" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G19" s="49"/>
       <c r="H19" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="I19" s="5"/>
+        <v>172</v>
+      </c>
+      <c r="I19" s="5">
+        <v>2.0</v>
+      </c>
       <c r="K19" s="5" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="N19" s="5">
         <v>2.0</v>
@@ -65978,28 +65937,28 @@
         <v>18.0</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="5" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="I20" s="5"/>
       <c r="K20" s="5" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="N20" s="5">
         <v>2.0</v>
@@ -66010,28 +65969,28 @@
         <v>19.0</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="G21" s="49"/>
       <c r="H21" s="5" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="I21" s="5"/>
       <c r="K21" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="N21" s="5">
         <v>2.0</v>
@@ -66042,28 +66001,28 @@
         <v>20.0</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E22" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G22" s="49"/>
       <c r="H22" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I22" s="5"/>
       <c r="K22" s="5" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="N22" s="5">
         <v>2.0</v>
@@ -66074,28 +66033,28 @@
         <v>21.0</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E23" s="49" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="N23" s="5">
         <v>2.0</v>
@@ -66106,26 +66065,26 @@
         <v>22.0</v>
       </c>
       <c r="B24" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="5" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="I24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="N24" s="5">
         <v>2.0</v>
@@ -66136,26 +66095,26 @@
         <v>23.0</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C25" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="E25" s="49" t="s">
         <v>163</v>
-      </c>
-      <c r="D25" s="49" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="49" t="s">
-        <v>161</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="N25" s="5">
         <v>2.0</v>
@@ -66166,24 +66125,28 @@
         <v>24.0</v>
       </c>
       <c r="B26" s="49" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>181</v>
-      </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+        <v>185</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>164</v>
+      </c>
       <c r="G26" s="49"/>
       <c r="H26" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="N26" s="60">
+        <v>194</v>
+      </c>
+      <c r="N26" s="5">
         <v>1.0</v>
       </c>
     </row>
@@ -66191,18 +66154,26 @@
       <c r="A27" s="49">
         <v>25.0</v>
       </c>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
+      <c r="B27" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="E27" s="49" t="s">
+        <v>163</v>
+      </c>
       <c r="G27" s="49"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="K27" s="5"/>
       <c r="M27" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="N27" s="60">
+        <v>186</v>
+      </c>
+      <c r="N27" s="5">
         <v>1.0</v>
       </c>
     </row>
@@ -66219,9 +66190,9 @@
       <c r="I28" s="5"/>
       <c r="K28" s="5"/>
       <c r="M28" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="N28" s="60">
+        <v>190</v>
+      </c>
+      <c r="N28" s="5">
         <v>1.0</v>
       </c>
     </row>
@@ -66237,9 +66208,9 @@
       <c r="I29" s="5"/>
       <c r="K29" s="5"/>
       <c r="M29" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="N29" s="60">
+        <v>187</v>
+      </c>
+      <c r="N29" s="5">
         <v>1.0</v>
       </c>
     </row>
@@ -66255,9 +66226,9 @@
       <c r="I30" s="5"/>
       <c r="K30" s="5"/>
       <c r="M30" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="N30" s="60">
+        <v>193</v>
+      </c>
+      <c r="N30" s="5">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Game week 39 update
</commit_message>
<xml_diff>
--- a/data/latest_data_prev.xlsx
+++ b/data/latest_data_prev.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="/Pp+ozo03evYlou6yoD5gsDlZNBRXeQ/1Lr+yorJtuk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="EEodVdc5IGuKlN969ht/aakT3X6mHD8ZL0qnZqerYBs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="228">
   <si>
     <t>MARLOW DUKES 2025</t>
   </si>
@@ -201,16 +201,19 @@
     <t>%</t>
   </si>
   <si>
-    <t>ZIGZAG</t>
+    <t>POSH CHRIS</t>
   </si>
   <si>
-    <t>POSH CHRIS</t>
+    <t>ZIGZAG</t>
   </si>
   <si>
     <t>BRUCE</t>
   </si>
   <si>
     <t>DUNCAN</t>
+  </si>
+  <si>
+    <t>FATHER TED</t>
   </si>
   <si>
     <t>IAN</t>
@@ -220,9 +223,6 @@
   </si>
   <si>
     <t>CARLOS</t>
-  </si>
-  <si>
-    <t>FATHER TED</t>
   </si>
   <si>
     <t>KERMIT</t>
@@ -237,16 +237,16 @@
     <t>WILSON</t>
   </si>
   <si>
+    <t xml:space="preserve">MAMAS </t>
+  </si>
+  <si>
+    <t>PRESTON</t>
+  </si>
+  <si>
     <t>DWARF</t>
   </si>
   <si>
-    <t xml:space="preserve">MAMAS </t>
-  </si>
-  <si>
     <t>INSPECTOR GADGET</t>
-  </si>
-  <si>
-    <t>PRESTON</t>
   </si>
   <si>
     <t>CAPTAIN KIRK</t>
@@ -258,13 +258,13 @@
     <t>SONES</t>
   </si>
   <si>
+    <t>KRYTON</t>
+  </si>
+  <si>
     <t>TOY BOY</t>
   </si>
   <si>
     <t>PHANTOM</t>
-  </si>
-  <si>
-    <t>KRYTON</t>
   </si>
   <si>
     <t>BANKSY</t>
@@ -543,10 +543,10 @@
     <t>ZigZag</t>
   </si>
   <si>
-    <t>Preston</t>
+    <t>Carlos</t>
   </si>
   <si>
-    <t>Carlos</t>
+    <t>Preston</t>
   </si>
   <si>
     <t>Duncan - Dom</t>
@@ -663,6 +663,9 @@
     <t>Gadget - Father Ted</t>
   </si>
   <si>
+    <t>Phantom</t>
+  </si>
+  <si>
     <t>Banksy - Preston</t>
   </si>
   <si>
@@ -700,6 +703,9 @@
   </si>
   <si>
     <t>Tango - Bruce</t>
+  </si>
+  <si>
+    <t>Ian - Father Ted</t>
   </si>
 </sst>
 </file>
@@ -1729,40 +1735,40 @@
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16">
-        <v>-1.0</v>
-      </c>
-      <c r="D5" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="G5" s="17">
         <v>3.0</v>
-      </c>
-      <c r="E5" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="16">
-        <v>-2.0</v>
-      </c>
-      <c r="G5" s="16">
-        <v>-3.0</v>
       </c>
       <c r="H5" s="16">
         <v>-3.0</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="16"/>
+      <c r="J5" s="16">
         <v>-2.0</v>
       </c>
-      <c r="J5" s="16"/>
       <c r="K5" s="15"/>
       <c r="L5" s="16">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="M5" s="16">
         <v>1.0</v>
       </c>
-      <c r="N5" s="16"/>
+      <c r="N5" s="16">
+        <v>2.0</v>
+      </c>
       <c r="O5" s="16">
         <v>1.0</v>
       </c>
-      <c r="P5" s="16">
-        <v>-1.0</v>
+      <c r="P5" s="17">
+        <v>1.0</v>
       </c>
       <c r="Q5" s="16">
         <v>2.0</v>
@@ -1770,41 +1776,35 @@
       <c r="R5" s="16">
         <v>0.0</v>
       </c>
-      <c r="S5" s="17">
-        <v>-2.0</v>
+      <c r="S5" s="16">
+        <v>2.0</v>
       </c>
       <c r="T5" s="16">
         <v>3.0</v>
       </c>
-      <c r="U5" s="16">
-        <v>0.0</v>
-      </c>
+      <c r="U5" s="16"/>
       <c r="V5" s="16">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="W5" s="15"/>
-      <c r="X5" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="Y5" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="Z5" s="16">
-        <v>2.0</v>
-      </c>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="17">
+        <v>-1.0</v>
+      </c>
+      <c r="Z5" s="16"/>
       <c r="AA5" s="16">
         <v>3.0</v>
       </c>
       <c r="AB5" s="16">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="AC5" s="16">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AD5" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="AE5" s="17">
+        <v>-5.0</v>
+      </c>
+      <c r="AE5" s="16">
         <v>0.0</v>
       </c>
       <c r="AF5" s="16">
@@ -1813,22 +1813,22 @@
       <c r="AG5" s="16">
         <v>0.0</v>
       </c>
-      <c r="AH5" s="16">
+      <c r="AH5" s="17">
         <v>2.0</v>
       </c>
       <c r="AI5" s="16">
         <v>3.0</v>
       </c>
-      <c r="AJ5" s="16">
-        <v>-3.0</v>
-      </c>
+      <c r="AJ5" s="16"/>
       <c r="AK5" s="16">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AL5" s="16">
         <v>-1.0</v>
       </c>
-      <c r="AM5" s="16"/>
+      <c r="AM5" s="16">
+        <v>1.0</v>
+      </c>
       <c r="AN5" s="16"/>
       <c r="AO5" s="16"/>
       <c r="AP5" s="16"/>
@@ -1845,31 +1845,31 @@
       </c>
       <c r="AZ5" s="5">
         <f t="shared" ref="AZ5:AZ40" si="1">COUNT(B5:AX5)</f>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="BA5" s="5">
         <f t="shared" ref="BA5:BA40" si="2">COUNTIF($B5:$AX5, "&gt;=1")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BB5" s="5">
         <f t="shared" ref="BB5:BB40" si="3">COUNTIF($B5:$AX5, "0")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC5" s="5">
         <f t="shared" ref="BC5:BC40" si="4">COUNTIF($B5:$AX5, "&lt;0")</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BD5" s="5">
         <f t="shared" ref="BD5:BD40" si="5">SUM(BA5*3)+BB5</f>
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="BE5" s="5">
         <f t="shared" ref="BE5:BE40" si="6">SUM(B5:AX5)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BF5" s="19">
         <f t="shared" ref="BF5:BF40" si="7">SUM(BA5*3+BB5*1)/SUM(AZ5*3)</f>
-        <v>0.5520833333</v>
+        <v>0.632183908</v>
       </c>
       <c r="BG5" s="19"/>
     </row>
@@ -1879,40 +1879,40 @@
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22">
+        <v>-1.0</v>
+      </c>
+      <c r="D6" s="22">
+        <v>3.0</v>
+      </c>
+      <c r="E6" s="23">
         <v>0.0</v>
       </c>
       <c r="F6" s="22">
-        <v>2.0</v>
-      </c>
-      <c r="G6" s="23">
-        <v>3.0</v>
+        <v>-2.0</v>
+      </c>
+      <c r="G6" s="22">
+        <v>-3.0</v>
       </c>
       <c r="H6" s="22">
         <v>-3.0</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22">
+      <c r="I6" s="22">
         <v>-2.0</v>
       </c>
+      <c r="J6" s="22"/>
       <c r="K6" s="21"/>
       <c r="L6" s="22">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="M6" s="22">
         <v>1.0</v>
       </c>
-      <c r="N6" s="22">
-        <v>2.0</v>
-      </c>
+      <c r="N6" s="22"/>
       <c r="O6" s="22">
         <v>1.0</v>
       </c>
-      <c r="P6" s="23">
-        <v>1.0</v>
+      <c r="P6" s="22">
+        <v>-1.0</v>
       </c>
       <c r="Q6" s="22">
         <v>2.0</v>
@@ -1920,35 +1920,41 @@
       <c r="R6" s="22">
         <v>0.0</v>
       </c>
-      <c r="S6" s="22">
-        <v>2.0</v>
+      <c r="S6" s="23">
+        <v>-2.0</v>
       </c>
       <c r="T6" s="22">
         <v>3.0</v>
       </c>
-      <c r="U6" s="22"/>
+      <c r="U6" s="22">
+        <v>0.0</v>
+      </c>
       <c r="V6" s="22">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="W6" s="21"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="23">
-        <v>-1.0</v>
-      </c>
-      <c r="Z6" s="22"/>
+      <c r="X6" s="22">
+        <v>2.0</v>
+      </c>
+      <c r="Y6" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="Z6" s="22">
+        <v>2.0</v>
+      </c>
       <c r="AA6" s="22">
         <v>3.0</v>
       </c>
       <c r="AB6" s="22">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="AC6" s="22">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AD6" s="22">
-        <v>-5.0</v>
-      </c>
-      <c r="AE6" s="22">
+        <v>5.0</v>
+      </c>
+      <c r="AE6" s="23">
         <v>0.0</v>
       </c>
       <c r="AF6" s="22">
@@ -1957,20 +1963,24 @@
       <c r="AG6" s="22">
         <v>0.0</v>
       </c>
-      <c r="AH6" s="23">
+      <c r="AH6" s="22">
         <v>2.0</v>
       </c>
       <c r="AI6" s="22">
         <v>3.0</v>
       </c>
-      <c r="AJ6" s="22"/>
+      <c r="AJ6" s="22">
+        <v>-3.0</v>
+      </c>
       <c r="AK6" s="22">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AL6" s="22">
         <v>-1.0</v>
       </c>
-      <c r="AM6" s="22"/>
+      <c r="AM6" s="22">
+        <v>-1.0</v>
+      </c>
       <c r="AN6" s="22"/>
       <c r="AO6" s="22"/>
       <c r="AP6" s="22"/>
@@ -1987,7 +1997,7 @@
       </c>
       <c r="AZ6" s="5">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="BA6" s="5">
         <f t="shared" si="2"/>
@@ -1995,23 +2005,23 @@
       </c>
       <c r="BB6" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BC6" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="BD6" s="5">
         <f t="shared" si="5"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BE6" s="5">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="BF6" s="19">
         <f t="shared" si="7"/>
-        <v>0.619047619</v>
+        <v>0.5353535354</v>
       </c>
       <c r="BG6" s="19"/>
     </row>
@@ -2118,7 +2128,9 @@
       <c r="AL7" s="27">
         <v>1.0</v>
       </c>
-      <c r="AM7" s="26"/>
+      <c r="AM7" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AN7" s="26"/>
       <c r="AO7" s="26"/>
       <c r="AP7" s="26"/>
@@ -2135,7 +2147,7 @@
       </c>
       <c r="AZ7" s="5">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BA7" s="5">
         <f t="shared" si="2"/>
@@ -2147,7 +2159,7 @@
       </c>
       <c r="BC7" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BD7" s="5">
         <f t="shared" si="5"/>
@@ -2155,11 +2167,11 @@
       </c>
       <c r="BE7" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF7" s="19">
         <f t="shared" si="7"/>
-        <v>0.5268817204</v>
+        <v>0.5104166667</v>
       </c>
       <c r="BG7" s="19"/>
     </row>
@@ -2266,7 +2278,9 @@
       <c r="AL8" s="16">
         <v>-1.0</v>
       </c>
-      <c r="AM8" s="16"/>
+      <c r="AM8" s="16">
+        <v>-1.0</v>
+      </c>
       <c r="AN8" s="16"/>
       <c r="AO8" s="16"/>
       <c r="AP8" s="16"/>
@@ -2283,7 +2297,7 @@
       </c>
       <c r="AZ8" s="5">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BA8" s="5">
         <f t="shared" si="2"/>
@@ -2295,7 +2309,7 @@
       </c>
       <c r="BC8" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BD8" s="5">
         <f t="shared" si="5"/>
@@ -2303,11 +2317,11 @@
       </c>
       <c r="BE8" s="5">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF8" s="19">
         <f t="shared" si="7"/>
-        <v>0.4946236559</v>
+        <v>0.4791666667</v>
       </c>
       <c r="BG8" s="19"/>
     </row>
@@ -2316,9 +2330,7 @@
         <v>63</v>
       </c>
       <c r="B9" s="29"/>
-      <c r="C9" s="30">
-        <v>-1.0</v>
-      </c>
+      <c r="C9" s="30"/>
       <c r="D9" s="30">
         <v>-3.0</v>
       </c>
@@ -2328,20 +2340,22 @@
       <c r="F9" s="30">
         <v>-2.0</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="31">
         <v>-3.0</v>
       </c>
       <c r="H9" s="30">
         <v>3.0</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="30">
         <v>-2.0</v>
       </c>
       <c r="J9" s="30">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="K9" s="29"/>
-      <c r="L9" s="30"/>
+      <c r="L9" s="30">
+        <v>-3.0</v>
+      </c>
       <c r="M9" s="30">
         <v>1.0</v>
       </c>
@@ -2349,13 +2363,13 @@
         <v>-2.0</v>
       </c>
       <c r="O9" s="30">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="P9" s="30"/>
-      <c r="Q9" s="31">
+      <c r="Q9" s="30">
         <v>-2.0</v>
       </c>
-      <c r="R9" s="30">
+      <c r="R9" s="31">
         <v>0.0</v>
       </c>
       <c r="S9" s="30">
@@ -2377,44 +2391,40 @@
       <c r="Y9" s="30">
         <v>1.0</v>
       </c>
-      <c r="Z9" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AA9" s="31">
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30">
         <v>3.0</v>
       </c>
-      <c r="AB9" s="30">
-        <v>-3.0</v>
+      <c r="AB9" s="31">
+        <v>3.0</v>
       </c>
       <c r="AC9" s="30">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AD9" s="30">
         <v>-5.0</v>
       </c>
-      <c r="AE9" s="30">
-        <v>0.0</v>
-      </c>
+      <c r="AE9" s="30"/>
       <c r="AF9" s="30">
         <v>1.0</v>
       </c>
-      <c r="AG9" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AH9" s="30"/>
-      <c r="AI9" s="30">
-        <v>3.0</v>
-      </c>
+      <c r="AG9" s="30"/>
+      <c r="AH9" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="AI9" s="30"/>
       <c r="AJ9" s="30">
         <v>3.0</v>
       </c>
       <c r="AK9" s="30">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AL9" s="30">
         <v>-1.0</v>
       </c>
-      <c r="AM9" s="30"/>
+      <c r="AM9" s="31">
+        <v>1.0</v>
+      </c>
       <c r="AN9" s="30"/>
       <c r="AO9" s="30"/>
       <c r="AP9" s="30"/>
@@ -2431,23 +2441,23 @@
       </c>
       <c r="AZ9" s="5">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="BA9" s="5">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BB9" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BC9" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BD9" s="5">
         <f t="shared" si="5"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="BE9" s="5">
         <f t="shared" si="6"/>
@@ -2455,7 +2465,7 @@
       </c>
       <c r="BF9" s="19">
         <f t="shared" si="7"/>
-        <v>0.4731182796</v>
+        <v>0.5172413793</v>
       </c>
       <c r="BG9" s="19"/>
     </row>
@@ -2465,14 +2475,16 @@
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="30">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D10" s="30">
         <v>-3.0</v>
       </c>
-      <c r="E10" s="30"/>
+      <c r="E10" s="30">
+        <v>0.0</v>
+      </c>
       <c r="F10" s="30">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G10" s="30">
         <v>-3.0</v>
@@ -2480,79 +2492,89 @@
       <c r="H10" s="30">
         <v>3.0</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="31">
+        <v>-2.0</v>
+      </c>
+      <c r="J10" s="30">
         <v>2.0</v>
       </c>
-      <c r="J10" s="31">
-        <v>2.0</v>
-      </c>
       <c r="K10" s="29"/>
-      <c r="L10" s="30">
-        <v>3.0</v>
-      </c>
+      <c r="L10" s="30"/>
       <c r="M10" s="30">
         <v>1.0</v>
       </c>
       <c r="N10" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="O10" s="26">
         <v>-1.0</v>
       </c>
-      <c r="P10" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Q10" s="26">
+      <c r="P10" s="26"/>
+      <c r="Q10" s="27">
         <v>-2.0</v>
       </c>
       <c r="R10" s="30">
         <v>0.0</v>
       </c>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="31">
+      <c r="S10" s="30">
+        <v>-2.0</v>
+      </c>
+      <c r="T10" s="30">
+        <v>3.0</v>
+      </c>
+      <c r="U10" s="30">
         <v>0.0</v>
       </c>
-      <c r="V10" s="30"/>
+      <c r="V10" s="30">
+        <v>1.0</v>
+      </c>
       <c r="W10" s="29"/>
       <c r="X10" s="30">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="Y10" s="30">
-        <v>-1.0</v>
-      </c>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30">
-        <v>-3.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="Z10" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="AA10" s="31">
+        <v>3.0</v>
       </c>
       <c r="AB10" s="30">
         <v>-3.0</v>
       </c>
       <c r="AC10" s="30">
+        <v>-1.0</v>
+      </c>
+      <c r="AD10" s="30">
+        <v>-5.0</v>
+      </c>
+      <c r="AE10" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="AF10" s="30">
         <v>1.0</v>
-      </c>
-      <c r="AD10" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="30">
-        <v>-1.0</v>
       </c>
       <c r="AG10" s="30">
         <v>0.0</v>
       </c>
-      <c r="AH10" s="31">
-        <v>-2.0</v>
-      </c>
+      <c r="AH10" s="30"/>
       <c r="AI10" s="30">
         <v>3.0</v>
       </c>
       <c r="AJ10" s="30">
         <v>3.0</v>
       </c>
-      <c r="AK10" s="30"/>
-      <c r="AL10" s="30"/>
-      <c r="AM10" s="30"/>
+      <c r="AK10" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="AL10" s="30">
+        <v>-1.0</v>
+      </c>
+      <c r="AM10" s="31">
+        <v>-1.0</v>
+      </c>
       <c r="AN10" s="30"/>
       <c r="AO10" s="30"/>
       <c r="AP10" s="30"/>
@@ -2569,7 +2591,7 @@
       </c>
       <c r="AZ10" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="BA10" s="5">
         <f t="shared" si="2"/>
@@ -2577,23 +2599,23 @@
       </c>
       <c r="BB10" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BC10" s="5">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>-3</v>
       </c>
       <c r="BF10" s="19">
         <f t="shared" si="7"/>
-        <v>0.5384615385</v>
+        <v>0.4583333333</v>
       </c>
       <c r="BG10" s="19"/>
     </row>
@@ -2606,70 +2628,68 @@
         <v>1.0</v>
       </c>
       <c r="D11" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="E11" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="27">
-        <v>-2.0</v>
+        <v>-3.0</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26">
+        <v>2.0</v>
       </c>
       <c r="G11" s="26">
         <v>-3.0</v>
       </c>
       <c r="H11" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="I11" s="26">
         <v>2.0</v>
       </c>
-      <c r="J11" s="26">
-        <v>-2.0</v>
+      <c r="J11" s="27">
+        <v>2.0</v>
       </c>
       <c r="K11" s="25"/>
-      <c r="L11" s="26"/>
+      <c r="L11" s="26">
+        <v>3.0</v>
+      </c>
       <c r="M11" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="N11" s="26">
         <v>2.0</v>
       </c>
-      <c r="O11" s="27">
+      <c r="O11" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="P11" s="26">
         <v>1.0</v>
       </c>
-      <c r="P11" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="Q11" s="26"/>
+      <c r="Q11" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="R11" s="26">
         <v>0.0</v>
       </c>
-      <c r="S11" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="T11" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="U11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="27">
+        <v>0.0</v>
+      </c>
       <c r="V11" s="26"/>
       <c r="W11" s="25"/>
       <c r="X11" s="26">
         <v>-2.0</v>
       </c>
       <c r="Y11" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AB11" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AC11" s="26">
         <v>1.0</v>
-      </c>
-      <c r="Z11" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="AA11" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="AB11" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AC11" s="26">
-        <v>-1.0</v>
       </c>
       <c r="AD11" s="26">
         <v>5.0</v>
@@ -2681,21 +2701,17 @@
       <c r="AG11" s="26">
         <v>0.0</v>
       </c>
-      <c r="AH11" s="26">
-        <v>2.0</v>
+      <c r="AH11" s="27">
+        <v>-2.0</v>
       </c>
       <c r="AI11" s="26">
         <v>3.0</v>
       </c>
-      <c r="AJ11" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="AK11" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AL11" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AJ11" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="AK11" s="26"/>
+      <c r="AL11" s="26"/>
       <c r="AM11" s="26"/>
       <c r="AN11" s="26"/>
       <c r="AO11" s="26"/>
@@ -2713,7 +2729,7 @@
       </c>
       <c r="AZ11" s="5">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="BA11" s="5">
         <f t="shared" si="2"/>
@@ -2725,7 +2741,7 @@
       </c>
       <c r="BC11" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="5"/>
@@ -2733,11 +2749,11 @@
       </c>
       <c r="BE11" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BF11" s="19">
         <f t="shared" si="7"/>
-        <v>0.4827586207</v>
+        <v>0.5384615385</v>
       </c>
       <c r="BG11" s="19"/>
     </row>
@@ -2746,97 +2762,99 @@
         <v>66</v>
       </c>
       <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
+      <c r="C12" s="26">
+        <v>1.0</v>
+      </c>
       <c r="D12" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="E12" s="26">
         <v>0.0</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="27">
         <v>-2.0</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="26">
         <v>-3.0</v>
       </c>
       <c r="H12" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I12" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="J12" s="26">
         <v>-2.0</v>
       </c>
       <c r="K12" s="25"/>
-      <c r="L12" s="26">
+      <c r="L12" s="26"/>
+      <c r="M12" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="N12" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="O12" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="P12" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="S12" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="T12" s="26">
         <v>-3.0</v>
       </c>
-      <c r="M12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="N12" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="O12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="R12" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="S12" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="T12" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="U12" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="V12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
       <c r="W12" s="25"/>
       <c r="X12" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="Y12" s="26">
         <v>1.0</v>
       </c>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26">
+      <c r="Z12" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="AA12" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="AB12" s="26">
         <v>3.0</v>
       </c>
-      <c r="AB12" s="27">
-        <v>3.0</v>
-      </c>
       <c r="AC12" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AD12" s="26">
-        <v>-5.0</v>
+        <v>5.0</v>
       </c>
       <c r="AE12" s="26"/>
       <c r="AF12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AG12" s="26"/>
+        <v>-1.0</v>
+      </c>
+      <c r="AG12" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH12" s="26">
         <v>2.0</v>
       </c>
-      <c r="AI12" s="26"/>
-      <c r="AJ12" s="26">
+      <c r="AI12" s="26">
         <v>3.0</v>
       </c>
+      <c r="AJ12" s="27">
+        <v>-3.0</v>
+      </c>
       <c r="AK12" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AL12" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AM12" s="26"/>
       <c r="AN12" s="26"/>
@@ -2855,7 +2873,7 @@
       </c>
       <c r="AZ12" s="5">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BA12" s="5">
         <f t="shared" si="2"/>
@@ -2867,7 +2885,7 @@
       </c>
       <c r="BC12" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BD12" s="5">
         <f t="shared" si="5"/>
@@ -2875,11 +2893,11 @@
       </c>
       <c r="BE12" s="5">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="BF12" s="19">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.4827586207</v>
       </c>
       <c r="BG12" s="19"/>
     </row>
@@ -2982,7 +3000,9 @@
       </c>
       <c r="AK13" s="26"/>
       <c r="AL13" s="26"/>
-      <c r="AM13" s="26"/>
+      <c r="AM13" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN13" s="26"/>
       <c r="AO13" s="26"/>
       <c r="AP13" s="26"/>
@@ -2999,11 +3019,11 @@
       </c>
       <c r="AZ13" s="5">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="BA13" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB13" s="5">
         <f t="shared" si="3"/>
@@ -3015,15 +3035,15 @@
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="5"/>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="BE13" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF13" s="19">
         <f t="shared" si="7"/>
-        <v>0.4367816092</v>
+        <v>0.4555555556</v>
       </c>
       <c r="BG13" s="19"/>
     </row>
@@ -3120,7 +3140,9 @@
       </c>
       <c r="AK14" s="26"/>
       <c r="AL14" s="26"/>
-      <c r="AM14" s="26"/>
+      <c r="AM14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN14" s="26"/>
       <c r="AO14" s="26"/>
       <c r="AP14" s="26"/>
@@ -3137,11 +3159,11 @@
       </c>
       <c r="AZ14" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BA14" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB14" s="5">
         <f t="shared" si="3"/>
@@ -3153,15 +3175,15 @@
       </c>
       <c r="BD14" s="5">
         <f t="shared" si="5"/>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="BE14" s="5">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BF14" s="19">
         <f t="shared" si="7"/>
-        <v>0.4743589744</v>
+        <v>0.4938271605</v>
       </c>
       <c r="BG14" s="19"/>
     </row>
@@ -3252,7 +3274,9 @@
       <c r="AL15" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM15" s="26"/>
+      <c r="AM15" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN15" s="26"/>
       <c r="AO15" s="26"/>
       <c r="AP15" s="26"/>
@@ -3269,11 +3293,11 @@
       </c>
       <c r="AZ15" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BA15" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB15" s="5">
         <f t="shared" si="3"/>
@@ -3285,15 +3309,15 @@
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="BE15" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BF15" s="19">
         <f t="shared" si="7"/>
-        <v>0.5217391304</v>
+        <v>0.5416666667</v>
       </c>
       <c r="BG15" s="19"/>
     </row>
@@ -3390,7 +3414,9 @@
         <v>-1.0</v>
       </c>
       <c r="AL16" s="26"/>
-      <c r="AM16" s="26"/>
+      <c r="AM16" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN16" s="26"/>
       <c r="AO16" s="26"/>
       <c r="AP16" s="26"/>
@@ -3407,11 +3433,11 @@
       </c>
       <c r="AZ16" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BA16" s="5">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BB16" s="5">
         <f t="shared" si="3"/>
@@ -3423,15 +3449,15 @@
       </c>
       <c r="BD16" s="5">
         <f t="shared" si="5"/>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="BE16" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF16" s="19">
         <f t="shared" si="7"/>
-        <v>0.4487179487</v>
+        <v>0.4691358025</v>
       </c>
       <c r="BG16" s="19"/>
     </row>
@@ -3440,31 +3466,35 @@
         <v>71</v>
       </c>
       <c r="B17" s="25"/>
-      <c r="C17" s="26">
+      <c r="C17" s="27">
         <v>-1.0</v>
       </c>
       <c r="D17" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="E17" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="G17" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="H17" s="26">
         <v>-3.0</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27">
-        <v>3.0</v>
-      </c>
       <c r="I17" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="J17" s="26">
         <v>-2.0</v>
-      </c>
-      <c r="J17" s="26">
-        <v>2.0</v>
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="26">
         <v>3.0</v>
       </c>
-      <c r="M17" s="26">
-        <v>-1.0</v>
-      </c>
+      <c r="M17" s="26"/>
       <c r="N17" s="26">
         <v>-2.0</v>
       </c>
@@ -3472,53 +3502,61 @@
         <v>1.0</v>
       </c>
       <c r="P17" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q17" s="26">
         <v>2.0</v>
       </c>
-      <c r="R17" s="26"/>
+      <c r="R17" s="26">
+        <v>0.0</v>
+      </c>
       <c r="S17" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="T17" s="26">
         <v>-3.0</v>
       </c>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26">
-        <v>-1.0</v>
+      <c r="U17" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="V17" s="27">
+        <v>1.0</v>
       </c>
       <c r="W17" s="25"/>
       <c r="X17" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="Y17" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="Z17" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="AA17" s="26">
-        <v>-3.0</v>
-      </c>
+        <v>-2.0</v>
+      </c>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="26"/>
       <c r="AB17" s="26"/>
       <c r="AC17" s="26"/>
       <c r="AD17" s="26"/>
       <c r="AE17" s="26">
         <v>0.0</v>
       </c>
-      <c r="AF17" s="26"/>
+      <c r="AF17" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AG17" s="26"/>
-      <c r="AH17" s="26"/>
-      <c r="AI17" s="27">
+      <c r="AH17" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="AI17" s="26">
         <v>3.0</v>
       </c>
-      <c r="AJ17" s="26"/>
-      <c r="AK17" s="26"/>
+      <c r="AJ17" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AK17" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AL17" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="AM17" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM17" s="26"/>
       <c r="AN17" s="26"/>
       <c r="AO17" s="26"/>
       <c r="AP17" s="26"/>
@@ -3535,7 +3573,7 @@
       </c>
       <c r="AZ17" s="5">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="BA17" s="5">
         <f t="shared" si="2"/>
@@ -3543,23 +3581,23 @@
       </c>
       <c r="BB17" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BC17" s="5">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="BE17" s="5">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="BF17" s="19">
         <f t="shared" si="7"/>
-        <v>0.5396825397</v>
+        <v>0.4567901235</v>
       </c>
       <c r="BG17" s="19"/>
     </row>
@@ -3568,20 +3606,20 @@
         <v>72</v>
       </c>
       <c r="B18" s="25"/>
-      <c r="C18" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="D18" s="26">
+      <c r="C18" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="27">
         <v>3.0</v>
       </c>
       <c r="E18" s="26">
         <v>0.0</v>
       </c>
       <c r="F18" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G18" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="H18" s="26">
         <v>-3.0</v>
@@ -3590,21 +3628,23 @@
         <v>2.0</v>
       </c>
       <c r="J18" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="K18" s="25"/>
       <c r="L18" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="M18" s="26"/>
+        <v>-3.0</v>
+      </c>
+      <c r="M18" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="N18" s="26">
         <v>-2.0</v>
       </c>
       <c r="O18" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="P18" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="Q18" s="26">
         <v>2.0</v>
@@ -3612,40 +3652,46 @@
       <c r="R18" s="26">
         <v>0.0</v>
       </c>
-      <c r="S18" s="26">
-        <v>-2.0</v>
-      </c>
+      <c r="S18" s="26"/>
       <c r="T18" s="26">
         <v>-3.0</v>
       </c>
       <c r="U18" s="26">
         <v>0.0</v>
       </c>
-      <c r="V18" s="27">
-        <v>1.0</v>
+      <c r="V18" s="26">
+        <v>-1.0</v>
       </c>
       <c r="W18" s="25"/>
       <c r="X18" s="26">
         <v>-2.0</v>
       </c>
       <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
+      <c r="Z18" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AA18" s="26"/>
       <c r="AB18" s="26"/>
-      <c r="AC18" s="26"/>
-      <c r="AD18" s="26"/>
+      <c r="AC18" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AD18" s="26">
+        <v>5.0</v>
+      </c>
       <c r="AE18" s="26">
         <v>0.0</v>
       </c>
-      <c r="AF18" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AG18" s="26"/>
+      <c r="AF18" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AG18" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH18" s="26">
         <v>-2.0</v>
       </c>
-      <c r="AI18" s="26">
-        <v>3.0</v>
+      <c r="AI18" s="27">
+        <v>-3.0</v>
       </c>
       <c r="AJ18" s="26">
         <v>-3.0</v>
@@ -3654,9 +3700,11 @@
         <v>-1.0</v>
       </c>
       <c r="AL18" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AM18" s="26"/>
+        <v>1.0</v>
+      </c>
+      <c r="AM18" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN18" s="26"/>
       <c r="AO18" s="26"/>
       <c r="AP18" s="26"/>
@@ -3673,7 +3721,7 @@
       </c>
       <c r="AZ18" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="BA18" s="5">
         <f t="shared" si="2"/>
@@ -3681,23 +3729,23 @@
       </c>
       <c r="BB18" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BC18" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="BD18" s="5">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="BE18" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-14</v>
       </c>
       <c r="BF18" s="19">
         <f t="shared" si="7"/>
-        <v>0.4358974359</v>
+        <v>0.376344086</v>
       </c>
       <c r="BG18" s="19"/>
     </row>
@@ -3713,13 +3761,11 @@
         <v>-3.0</v>
       </c>
       <c r="E19" s="26"/>
-      <c r="F19" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="G19" s="26">
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27">
         <v>3.0</v>
       </c>
-      <c r="H19" s="26"/>
       <c r="I19" s="26">
         <v>-2.0</v>
       </c>
@@ -3727,78 +3773,68 @@
         <v>2.0</v>
       </c>
       <c r="K19" s="25"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="27">
+      <c r="L19" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="M19" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="N19" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="O19" s="26">
         <v>1.0</v>
       </c>
-      <c r="N19" s="26">
+      <c r="P19" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="Q19" s="26">
         <v>2.0</v>
       </c>
-      <c r="O19" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="P19" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Q19" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="R19" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="R19" s="26"/>
       <c r="S19" s="26">
         <v>2.0</v>
       </c>
       <c r="T19" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="U19" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="V19" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26">
         <v>-1.0</v>
       </c>
       <c r="W19" s="25"/>
       <c r="X19" s="26">
         <v>2.0</v>
       </c>
-      <c r="Y19" s="26">
-        <v>-1.0</v>
+      <c r="Y19" s="27">
+        <v>1.0</v>
       </c>
       <c r="Z19" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="AA19" s="26">
         <v>-3.0</v>
       </c>
-      <c r="AB19" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="AC19" s="26">
+      <c r="AB19" s="26"/>
+      <c r="AC19" s="26"/>
+      <c r="AD19" s="26"/>
+      <c r="AE19" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="AF19" s="26"/>
+      <c r="AG19" s="26"/>
+      <c r="AH19" s="26"/>
+      <c r="AI19" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="AJ19" s="26"/>
+      <c r="AK19" s="26"/>
+      <c r="AL19" s="26">
         <v>1.0</v>
       </c>
-      <c r="AD19" s="26"/>
-      <c r="AE19" s="26"/>
-      <c r="AF19" s="26">
+      <c r="AM19" s="26">
         <v>-1.0</v>
       </c>
-      <c r="AG19" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="AH19" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="AI19" s="26"/>
-      <c r="AJ19" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AK19" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AL19" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AM19" s="26"/>
       <c r="AN19" s="26"/>
       <c r="AO19" s="26"/>
       <c r="AP19" s="26"/>
@@ -3815,31 +3851,31 @@
       </c>
       <c r="AZ19" s="5">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="BA19" s="5">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BB19" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BC19" s="5">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="BD19" s="5">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BE19" s="5">
         <f t="shared" si="6"/>
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="BF19" s="19">
         <f t="shared" si="7"/>
-        <v>0.3928571429</v>
+        <v>0.5151515152</v>
       </c>
       <c r="BG19" s="19"/>
     </row>
@@ -3849,82 +3885,80 @@
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="E20" s="26">
-        <v>0.0</v>
-      </c>
+        <v>-1.0</v>
+      </c>
+      <c r="D20" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="E20" s="26"/>
       <c r="F20" s="26">
         <v>-2.0</v>
       </c>
       <c r="G20" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="H20" s="26">
-        <v>-3.0</v>
-      </c>
+        <v>3.0</v>
+      </c>
+      <c r="H20" s="26"/>
       <c r="I20" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="J20" s="26">
         <v>2.0</v>
       </c>
       <c r="K20" s="25"/>
-      <c r="L20" s="26">
-        <v>-3.0</v>
-      </c>
+      <c r="L20" s="26"/>
       <c r="M20" s="27">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="N20" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="O20" s="26">
         <v>-1.0</v>
       </c>
       <c r="P20" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q20" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="R20" s="26">
         <v>0.0</v>
       </c>
-      <c r="S20" s="26"/>
+      <c r="S20" s="26">
+        <v>2.0</v>
+      </c>
       <c r="T20" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="U20" s="26">
         <v>0.0</v>
       </c>
-      <c r="V20" s="26">
+      <c r="V20" s="27">
         <v>-1.0</v>
       </c>
       <c r="W20" s="25"/>
       <c r="X20" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="Y20" s="26"/>
+        <v>2.0</v>
+      </c>
+      <c r="Y20" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="Z20" s="26">
         <v>-2.0</v>
       </c>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
-      <c r="AC20" s="27">
+      <c r="AA20" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AB20" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="AC20" s="26">
         <v>1.0</v>
       </c>
-      <c r="AD20" s="26">
-        <v>5.0</v>
-      </c>
-      <c r="AE20" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AD20" s="26"/>
+      <c r="AE20" s="26"/>
       <c r="AF20" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AG20" s="26">
         <v>0.0</v>
@@ -3932,19 +3966,19 @@
       <c r="AH20" s="26">
         <v>-2.0</v>
       </c>
-      <c r="AI20" s="27">
-        <v>-3.0</v>
-      </c>
+      <c r="AI20" s="26"/>
       <c r="AJ20" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="AK20" s="26">
         <v>-1.0</v>
       </c>
       <c r="AL20" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AM20" s="26"/>
+        <v>-1.0</v>
+      </c>
+      <c r="AM20" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AN20" s="26"/>
       <c r="AO20" s="26"/>
       <c r="AP20" s="26"/>
@@ -3961,15 +3995,15 @@
       </c>
       <c r="AZ20" s="5">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="BA20" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BB20" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BC20" s="5">
         <f t="shared" si="4"/>
@@ -3977,15 +4011,15 @@
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="6"/>
-        <v>-15</v>
+        <v>-7</v>
       </c>
       <c r="BF20" s="19">
         <f t="shared" si="7"/>
-        <v>0.3555555556</v>
+        <v>0.3793103448</v>
       </c>
       <c r="BG20" s="19"/>
     </row>
@@ -4176,7 +4210,9 @@
       <c r="AL22" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM22" s="26"/>
+      <c r="AM22" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AN22" s="26"/>
       <c r="AO22" s="26"/>
       <c r="AP22" s="26"/>
@@ -4193,7 +4229,7 @@
       </c>
       <c r="AZ22" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA22" s="5">
         <f t="shared" si="2"/>
@@ -4205,7 +4241,7 @@
       </c>
       <c r="BC22" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BD22" s="5">
         <f t="shared" si="5"/>
@@ -4213,11 +4249,11 @@
       </c>
       <c r="BE22" s="5">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BF22" s="19">
         <f t="shared" si="7"/>
-        <v>0.5897435897</v>
+        <v>0.5476190476</v>
       </c>
       <c r="BG22" s="19"/>
     </row>
@@ -4336,39 +4372,45 @@
         <v>78</v>
       </c>
       <c r="B24" s="25"/>
-      <c r="C24" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="E24" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="F24" s="26"/>
       <c r="G24" s="26">
         <v>3.0</v>
       </c>
       <c r="H24" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I24" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="J24" s="26"/>
       <c r="K24" s="25"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
+      <c r="L24" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="M24" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="N24" s="26"/>
       <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
+      <c r="P24" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="Q24" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="R24" s="26">
+        <v>0.0</v>
+      </c>
       <c r="S24" s="26"/>
-      <c r="T24" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="U24" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
       <c r="V24" s="26"/>
       <c r="W24" s="25"/>
       <c r="X24" s="26"/>
@@ -4382,11 +4424,21 @@
       <c r="AF24" s="26"/>
       <c r="AG24" s="26"/>
       <c r="AH24" s="26"/>
-      <c r="AI24" s="26"/>
-      <c r="AJ24" s="26"/>
-      <c r="AK24" s="26"/>
-      <c r="AL24" s="26"/>
-      <c r="AM24" s="26"/>
+      <c r="AI24" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AJ24" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AK24" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="AL24" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="AM24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN24" s="26"/>
       <c r="AO24" s="26"/>
       <c r="AP24" s="26"/>
@@ -4403,7 +4455,7 @@
       </c>
       <c r="AZ24" s="5">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="BA24" s="5">
         <f t="shared" si="2"/>
@@ -4411,23 +4463,23 @@
       </c>
       <c r="BB24" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC24" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="BD24" s="5">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BE24" s="5">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>-7</v>
       </c>
       <c r="BF24" s="19">
         <f t="shared" si="7"/>
-        <v>0.7619047619</v>
+        <v>0.3777777778</v>
       </c>
       <c r="BG24" s="19"/>
     </row>
@@ -4436,13 +4488,23 @@
         <v>79</v>
       </c>
       <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
+      <c r="C25" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
+      <c r="F25" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="G25" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="H25" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="I25" s="26">
+        <v>2.0</v>
+      </c>
       <c r="J25" s="26"/>
       <c r="K25" s="25"/>
       <c r="L25" s="26"/>
@@ -4453,39 +4515,29 @@
       <c r="Q25" s="26"/>
       <c r="R25" s="26"/>
       <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
+      <c r="T25" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="U25" s="26">
+        <v>0.0</v>
+      </c>
       <c r="V25" s="26"/>
       <c r="W25" s="25"/>
       <c r="X25" s="26"/>
       <c r="Y25" s="26"/>
       <c r="Z25" s="26"/>
       <c r="AA25" s="26"/>
-      <c r="AB25" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AC25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AB25" s="26"/>
+      <c r="AC25" s="26"/>
       <c r="AD25" s="26"/>
-      <c r="AE25" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AE25" s="26"/>
       <c r="AF25" s="26"/>
-      <c r="AG25" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AG25" s="26"/>
       <c r="AH25" s="26"/>
       <c r="AI25" s="26"/>
-      <c r="AJ25" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="AK25" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AL25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AJ25" s="26"/>
+      <c r="AK25" s="26"/>
+      <c r="AL25" s="26"/>
       <c r="AM25" s="26"/>
       <c r="AN25" s="26"/>
       <c r="AO25" s="26"/>
@@ -4507,11 +4559,11 @@
       </c>
       <c r="BA25" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB25" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC25" s="5">
         <f t="shared" si="4"/>
@@ -4519,15 +4571,15 @@
       </c>
       <c r="BD25" s="5">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BE25" s="5">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="BF25" s="19">
         <f t="shared" si="7"/>
-        <v>0.6666666667</v>
+        <v>0.7619047619</v>
       </c>
       <c r="BG25" s="19"/>
     </row>
@@ -4537,41 +4589,21 @@
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
-      <c r="D26" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="E26" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="26"/>
-      <c r="G26" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="H26" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="I26" s="26">
-        <v>-2.0</v>
-      </c>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
       <c r="J26" s="26"/>
       <c r="K26" s="25"/>
-      <c r="L26" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="M26" s="26">
-        <v>-1.0</v>
-      </c>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
       <c r="N26" s="26"/>
       <c r="O26" s="26"/>
-      <c r="P26" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Q26" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="R26" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
       <c r="S26" s="26"/>
       <c r="T26" s="26"/>
       <c r="U26" s="26"/>
@@ -4581,26 +4613,34 @@
       <c r="Y26" s="26"/>
       <c r="Z26" s="26"/>
       <c r="AA26" s="26"/>
-      <c r="AB26" s="26"/>
-      <c r="AC26" s="26"/>
+      <c r="AB26" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="AC26" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AD26" s="26"/>
-      <c r="AE26" s="26"/>
+      <c r="AE26" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AF26" s="26"/>
-      <c r="AG26" s="26"/>
+      <c r="AG26" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH26" s="26"/>
-      <c r="AI26" s="26">
-        <v>-3.0</v>
-      </c>
+      <c r="AI26" s="26"/>
       <c r="AJ26" s="26">
         <v>-3.0</v>
       </c>
-      <c r="AK26" s="27">
+      <c r="AK26" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AL26" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AM26" s="26">
         <v>-1.0</v>
       </c>
-      <c r="AL26" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AM26" s="26"/>
       <c r="AN26" s="26"/>
       <c r="AO26" s="26"/>
       <c r="AP26" s="26"/>
@@ -4617,7 +4657,7 @@
       </c>
       <c r="AZ26" s="5">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="BA26" s="5">
         <f t="shared" si="2"/>
@@ -4629,7 +4669,7 @@
       </c>
       <c r="BC26" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="BD26" s="5">
         <f t="shared" si="5"/>
@@ -4637,11 +4677,11 @@
       </c>
       <c r="BE26" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>2</v>
       </c>
       <c r="BF26" s="19">
         <f t="shared" si="7"/>
-        <v>0.3333333333</v>
+        <v>0.5833333333</v>
       </c>
       <c r="BG26" s="19"/>
     </row>
@@ -4726,7 +4766,9 @@
       <c r="AL27" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM27" s="26"/>
+      <c r="AM27" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AN27" s="26"/>
       <c r="AO27" s="26"/>
       <c r="AP27" s="26"/>
@@ -4743,7 +4785,7 @@
       </c>
       <c r="AZ27" s="5">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="BA27" s="5">
         <f t="shared" si="2"/>
@@ -4755,7 +4797,7 @@
       </c>
       <c r="BC27" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BD27" s="5">
         <f t="shared" si="5"/>
@@ -4763,11 +4805,11 @@
       </c>
       <c r="BE27" s="5">
         <f t="shared" si="6"/>
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="BF27" s="19">
         <f t="shared" si="7"/>
-        <v>0.2166666667</v>
+        <v>0.2063492063</v>
       </c>
       <c r="BG27" s="19"/>
     </row>
@@ -6137,7 +6179,7 @@
       </c>
       <c r="AM41" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AN41" s="30">
         <f t="shared" si="8"/>
@@ -6298,7 +6340,9 @@
       <c r="AL42" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="AM42" s="5"/>
+      <c r="AM42" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="AN42" s="5"/>
       <c r="AO42" s="5"/>
       <c r="AP42" s="5"/>
@@ -26603,7 +26647,7 @@
     </row>
     <row r="3">
       <c r="A3" s="40" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B3" s="41">
         <v>3.0</v>
@@ -26651,7 +26695,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="39">
         <v>4.0</v>
@@ -26675,33 +26719,33 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B6" s="39">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C6" s="39">
         <v>2.0</v>
       </c>
       <c r="D6" s="39">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" s="39">
         <v>1.0</v>
       </c>
       <c r="F6" s="39">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="G6" s="39">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I6" s="39">
         <v>18.0</v>
       </c>
       <c r="J6" s="42">
         <f t="shared" ref="J6:J10" si="2">I6/B6</f>
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="L6" s="34"/>
       <c r="M6" s="43"/>
@@ -26709,26 +26753,26 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B7" s="39">
         <v>3.0</v>
       </c>
       <c r="C7" s="39">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7" s="39">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E7" s="39">
         <v>1.0</v>
       </c>
       <c r="F7" s="39">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G7" s="39">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I7" s="39">
         <v>24.0</v>
@@ -26741,7 +26785,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B8" s="39">
         <v>3.0</v>
@@ -26756,7 +26800,7 @@
         <v>1.0</v>
       </c>
       <c r="F8" s="39">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G8" s="39">
         <f t="shared" si="1"/>
@@ -26772,7 +26816,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="39">
         <v>3.0</v>
@@ -26914,7 +26958,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="39">
         <v>1.0</v>
@@ -27066,19 +27110,19 @@
     </row>
     <row r="19">
       <c r="A19" s="32" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B19" s="39">
         <v>3.0</v>
       </c>
       <c r="C19" s="39">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D19" s="39">
+        <v>3.0</v>
+      </c>
+      <c r="E19" s="39">
         <v>0.0</v>
-      </c>
-      <c r="E19" s="39">
-        <v>2.0</v>
       </c>
       <c r="F19" s="39">
         <v>0.0</v>
@@ -27097,22 +27141,22 @@
     </row>
     <row r="20">
       <c r="A20" s="32" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="B20" s="39">
         <v>3.0</v>
       </c>
       <c r="C20" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="39">
         <v>0.0</v>
       </c>
-      <c r="D20" s="39">
-        <v>3.0</v>
-      </c>
       <c r="E20" s="39">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="F20" s="39">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G20" s="39">
         <f t="shared" si="1"/>
@@ -27129,10 +27173,10 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="32" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="B21" s="39">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C21" s="39">
         <v>1.0</v>
@@ -27141,7 +27185,7 @@
         <v>0.0</v>
       </c>
       <c r="E21" s="39">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F21" s="39">
         <v>-1.0</v>
@@ -27155,12 +27199,12 @@
       </c>
       <c r="J21" s="42">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="39">
         <v>3.0</v>
@@ -27256,7 +27300,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B25" s="39">
         <v>4.0</v>
@@ -27288,7 +27332,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B26" s="39">
         <v>3.0</v>
@@ -27374,7 +27418,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B29" s="39">
         <v>2.0</v>
@@ -28625,69 +28669,63 @@
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="16"/>
+        <v>73</v>
+      </c>
+      <c r="B3" s="15"/>
       <c r="C3" s="16">
         <v>1.0</v>
       </c>
-      <c r="D3" s="16">
-        <v>1.0</v>
-      </c>
+      <c r="D3" s="16"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="16">
-        <v>4.0</v>
-      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
       <c r="H3" s="16">
         <v>1.0</v>
       </c>
       <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="J3" s="16">
+        <v>1.0</v>
+      </c>
       <c r="K3" s="15"/>
       <c r="L3" s="16"/>
-      <c r="M3" s="16">
-        <v>1.0</v>
-      </c>
+      <c r="M3" s="16"/>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
+      <c r="Q3" s="16">
+        <v>3.0</v>
+      </c>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
       <c r="T3" s="16"/>
       <c r="U3" s="16"/>
-      <c r="V3" s="16">
+      <c r="V3" s="16"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="16">
+        <v>6.0</v>
+      </c>
+      <c r="Y3" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="Z3" s="16">
         <v>2.0</v>
       </c>
-      <c r="W3" s="15"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16">
-        <v>1.0</v>
-      </c>
       <c r="AA3" s="16"/>
-      <c r="AB3" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AC3" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AD3" s="16">
-        <v>3.0</v>
-      </c>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
       <c r="AE3" s="16"/>
       <c r="AF3" s="16"/>
       <c r="AG3" s="16"/>
-      <c r="AH3" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AI3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AJ3" s="16"/>
       <c r="AK3" s="16"/>
-      <c r="AL3" s="16"/>
+      <c r="AL3" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AM3" s="16"/>
       <c r="AN3" s="16"/>
       <c r="AO3" s="16"/>
@@ -28704,67 +28742,77 @@
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6">
         <f t="shared" ref="BA3:BA36" si="1">SUM(B3:AY3)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BB3" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC3" s="5"/>
+        <v>2.0</v>
+      </c>
+      <c r="BC3" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="29"/>
+        <v>62</v>
+      </c>
+      <c r="B4" s="30"/>
       <c r="C4" s="30">
         <v>1.0</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="30">
+        <v>1.0</v>
+      </c>
       <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+      <c r="F4" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="30">
+        <v>4.0</v>
+      </c>
       <c r="H4" s="30">
         <v>1.0</v>
       </c>
       <c r="I4" s="30"/>
-      <c r="J4" s="30">
-        <v>1.0</v>
-      </c>
+      <c r="J4" s="30"/>
       <c r="K4" s="29"/>
       <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
+      <c r="M4" s="30">
+        <v>1.0</v>
+      </c>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30"/>
-      <c r="Q4" s="30">
-        <v>3.0</v>
-      </c>
+      <c r="Q4" s="30"/>
       <c r="R4" s="30"/>
       <c r="S4" s="30"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
+      <c r="V4" s="30">
+        <v>2.0</v>
+      </c>
       <c r="W4" s="29"/>
-      <c r="X4" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="Y4" s="30">
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30">
         <v>1.0</v>
       </c>
-      <c r="Z4" s="30">
-        <v>2.0</v>
-      </c>
       <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
+      <c r="AB4" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="AC4" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="AD4" s="30">
+        <v>3.0</v>
+      </c>
       <c r="AE4" s="30"/>
       <c r="AF4" s="30"/>
       <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="30">
-        <v>2.0</v>
-      </c>
+      <c r="AH4" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="AI4" s="30"/>
       <c r="AJ4" s="30"/>
       <c r="AK4" s="30"/>
       <c r="AL4" s="30"/>
@@ -28784,18 +28832,16 @@
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BB4" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="BC4" s="5">
-        <v>2.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="BC4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="26">
@@ -28879,7 +28925,7 @@
     </row>
     <row r="6">
       <c r="A6" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
@@ -29121,61 +29167,57 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
+      <c r="C9" s="26">
+        <v>1.0</v>
+      </c>
       <c r="D9" s="26"/>
-      <c r="E9" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="E9" s="26"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
+      <c r="J9" s="26">
+        <v>2.0</v>
+      </c>
       <c r="K9" s="25"/>
       <c r="L9" s="26"/>
-      <c r="M9" s="26">
+      <c r="M9" s="26"/>
+      <c r="N9" s="26">
         <v>1.0</v>
       </c>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
+      <c r="O9" s="26">
+        <v>2.0</v>
+      </c>
       <c r="P9" s="26"/>
       <c r="Q9" s="26"/>
       <c r="R9" s="26"/>
-      <c r="S9" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="S9" s="26"/>
       <c r="T9" s="26"/>
       <c r="U9" s="26"/>
       <c r="V9" s="26"/>
       <c r="W9" s="25"/>
-      <c r="X9" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Y9" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
       <c r="Z9" s="26"/>
       <c r="AA9" s="26"/>
       <c r="AB9" s="26">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AC9" s="26"/>
       <c r="AD9" s="26"/>
-      <c r="AE9" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AE9" s="26"/>
       <c r="AF9" s="26"/>
       <c r="AG9" s="26"/>
       <c r="AH9" s="26"/>
       <c r="AI9" s="26"/>
       <c r="AJ9" s="26"/>
-      <c r="AK9" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="AL9" s="26"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="26">
+        <v>3.0</v>
+      </c>
       <c r="AM9" s="26"/>
       <c r="AN9" s="26"/>
       <c r="AO9" s="26"/>
@@ -29192,72 +29234,66 @@
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC9" s="5">
-        <v>2.0</v>
-      </c>
+        <v>3.0</v>
+      </c>
+      <c r="BC9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="25"/>
+        <v>72</v>
+      </c>
+      <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="26">
         <v>1.0</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
+      <c r="G10" s="26">
+        <v>1.0</v>
+      </c>
       <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
+      <c r="I10" s="26">
+        <v>7.0</v>
+      </c>
       <c r="J10" s="26"/>
       <c r="K10" s="25"/>
       <c r="L10" s="26"/>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
-      <c r="O10" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="O10" s="26"/>
       <c r="P10" s="26"/>
-      <c r="Q10" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="Q10" s="26"/>
       <c r="R10" s="26"/>
       <c r="S10" s="26"/>
       <c r="T10" s="26"/>
-      <c r="U10" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="V10" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
       <c r="W10" s="25"/>
       <c r="X10" s="26"/>
       <c r="Y10" s="26"/>
-      <c r="Z10" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="Z10" s="26"/>
       <c r="AA10" s="26"/>
       <c r="AB10" s="26"/>
-      <c r="AC10" s="26"/>
-      <c r="AD10" s="26">
+      <c r="AC10" s="26">
         <v>1.0</v>
       </c>
-      <c r="AE10" s="26"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AF10" s="26"/>
       <c r="AG10" s="26"/>
       <c r="AH10" s="26"/>
-      <c r="AI10" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AI10" s="26"/>
       <c r="AJ10" s="26"/>
       <c r="AK10" s="26"/>
-      <c r="AL10" s="26"/>
+      <c r="AL10" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AM10" s="26"/>
       <c r="AN10" s="26"/>
       <c r="AO10" s="26"/>
@@ -29274,39 +29310,37 @@
       <c r="AZ10" s="6"/>
       <c r="BA10" s="6">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB10" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC10" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="BC10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
-      <c r="D11" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="D11" s="26"/>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H11" s="26"/>
-      <c r="I11" s="26">
-        <v>7.0</v>
-      </c>
+      <c r="I11" s="26"/>
       <c r="J11" s="26"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="26"/>
+      <c r="L11" s="26">
+        <v>3.0</v>
+      </c>
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
+      <c r="O11" s="26">
+        <v>1.0</v>
+      </c>
       <c r="P11" s="26"/>
       <c r="Q11" s="26"/>
       <c r="R11" s="26"/>
@@ -29318,22 +29352,30 @@
       <c r="X11" s="26"/>
       <c r="Y11" s="26"/>
       <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
+      <c r="AA11" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AB11" s="26"/>
-      <c r="AC11" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AC11" s="26"/>
       <c r="AD11" s="26"/>
       <c r="AE11" s="26">
         <v>1.0</v>
       </c>
       <c r="AF11" s="26"/>
-      <c r="AG11" s="26"/>
-      <c r="AH11" s="26"/>
+      <c r="AG11" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AH11" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AI11" s="26"/>
       <c r="AJ11" s="26"/>
-      <c r="AK11" s="26"/>
-      <c r="AL11" s="26"/>
+      <c r="AK11" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AL11" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AM11" s="26"/>
       <c r="AN11" s="26"/>
       <c r="AO11" s="26"/>
@@ -29350,7 +29392,7 @@
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB11" s="5">
         <v>1.0</v>
@@ -29359,7 +29401,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="26"/>
@@ -29367,41 +29409,39 @@
       <c r="E12" s="26">
         <v>1.0</v>
       </c>
-      <c r="F12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="F12" s="26"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="H12" s="26"/>
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
       <c r="K12" s="25"/>
       <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
+      <c r="M12" s="26">
+        <v>1.0</v>
+      </c>
       <c r="N12" s="26"/>
-      <c r="O12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="O12" s="26"/>
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
-      <c r="R12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="U12" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
       <c r="V12" s="26"/>
       <c r="W12" s="25"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
+      <c r="X12" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="Y12" s="26">
+        <v>2.0</v>
+      </c>
       <c r="Z12" s="26"/>
       <c r="AA12" s="26"/>
-      <c r="AB12" s="26"/>
+      <c r="AB12" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AC12" s="26"/>
       <c r="AD12" s="26"/>
       <c r="AE12" s="26">
@@ -29410,11 +29450,11 @@
       <c r="AF12" s="26"/>
       <c r="AG12" s="26"/>
       <c r="AH12" s="26"/>
-      <c r="AI12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AI12" s="26"/>
       <c r="AJ12" s="26"/>
-      <c r="AK12" s="26"/>
+      <c r="AK12" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AL12" s="26"/>
       <c r="AM12" s="26"/>
       <c r="AN12" s="26"/>
@@ -29437,64 +29477,66 @@
       <c r="BB12" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC12" s="5"/>
+      <c r="BC12" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="D13" s="26">
+        <v>1.0</v>
+      </c>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
-      <c r="G13" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="G13" s="26"/>
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="L13" s="26"/>
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26">
         <v>1.0</v>
       </c>
       <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
+      <c r="Q13" s="26">
+        <v>1.0</v>
+      </c>
       <c r="R13" s="26"/>
       <c r="S13" s="26"/>
       <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="26"/>
+      <c r="U13" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="V13" s="26">
+        <v>3.0</v>
+      </c>
       <c r="W13" s="25"/>
       <c r="X13" s="26"/>
       <c r="Y13" s="26"/>
-      <c r="Z13" s="26"/>
-      <c r="AA13" s="26">
+      <c r="Z13" s="26">
         <v>1.0</v>
       </c>
+      <c r="AA13" s="26"/>
       <c r="AB13" s="26"/>
       <c r="AC13" s="26"/>
-      <c r="AD13" s="26"/>
-      <c r="AE13" s="26">
+      <c r="AD13" s="26">
         <v>1.0</v>
       </c>
+      <c r="AE13" s="26"/>
       <c r="AF13" s="26"/>
-      <c r="AG13" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AH13" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AI13" s="26"/>
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26"/>
+      <c r="AI13" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AJ13" s="26"/>
-      <c r="AK13" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AK13" s="26"/>
       <c r="AL13" s="26"/>
       <c r="AM13" s="26"/>
       <c r="AN13" s="26"/>
@@ -29517,57 +29559,67 @@
       <c r="BB13" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC13" s="5"/>
+      <c r="BC13" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BF13" s="6"/>
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B14" s="25"/>
-      <c r="C14" s="26">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26">
         <v>1.0</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="F14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
+      <c r="H14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="I14" s="26"/>
-      <c r="J14" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="J14" s="26"/>
       <c r="K14" s="25"/>
       <c r="L14" s="26"/>
       <c r="M14" s="26"/>
-      <c r="N14" s="26">
+      <c r="N14" s="26"/>
+      <c r="O14" s="26">
         <v>1.0</v>
-      </c>
-      <c r="O14" s="26">
-        <v>2.0</v>
       </c>
       <c r="P14" s="26"/>
       <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
+      <c r="R14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
+      <c r="T14" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="U14" s="26">
+        <v>3.0</v>
+      </c>
       <c r="V14" s="26"/>
       <c r="W14" s="25"/>
       <c r="X14" s="26"/>
       <c r="Y14" s="26"/>
       <c r="Z14" s="26"/>
       <c r="AA14" s="26"/>
-      <c r="AB14" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="AB14" s="26"/>
       <c r="AC14" s="26"/>
       <c r="AD14" s="26"/>
-      <c r="AE14" s="26"/>
+      <c r="AE14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AF14" s="26"/>
       <c r="AG14" s="26"/>
       <c r="AH14" s="26"/>
-      <c r="AI14" s="26"/>
+      <c r="AI14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AJ14" s="26"/>
       <c r="AK14" s="26"/>
       <c r="AL14" s="26"/>
@@ -29587,10 +29639,10 @@
       <c r="AZ14" s="6"/>
       <c r="BA14" s="6">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BB14" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="BC14" s="5"/>
     </row>
@@ -29975,7 +30027,7 @@
     </row>
     <row r="20">
       <c r="A20" s="32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="26"/>
@@ -30054,14 +30106,16 @@
         <v>78</v>
       </c>
       <c r="B21" s="25"/>
-      <c r="C21" s="26">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26">
         <v>2.0</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
+      <c r="H21" s="26">
+        <v>2.0</v>
+      </c>
       <c r="I21" s="26"/>
       <c r="J21" s="26"/>
       <c r="K21" s="25"/>
@@ -30071,14 +30125,12 @@
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
+      <c r="R21" s="26">
+        <v>2.0</v>
+      </c>
       <c r="S21" s="26"/>
-      <c r="T21" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="U21" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="25"/>
       <c r="X21" s="26"/>
@@ -30095,7 +30147,9 @@
       <c r="AI21" s="26"/>
       <c r="AJ21" s="26"/>
       <c r="AK21" s="26"/>
-      <c r="AL21" s="26"/>
+      <c r="AL21" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AM21" s="26"/>
       <c r="AN21" s="26"/>
       <c r="AO21" s="26"/>
@@ -30114,17 +30168,21 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="BB21" s="5"/>
+      <c r="BB21" s="5">
+        <v>2.0</v>
+      </c>
       <c r="BC21" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="32" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="C22" s="26">
+        <v>2.0</v>
+      </c>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
       <c r="F22" s="26"/>
@@ -30141,29 +30199,27 @@
       <c r="Q22" s="26"/>
       <c r="R22" s="26"/>
       <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
+      <c r="T22" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="U22" s="26">
+        <v>2.0</v>
+      </c>
       <c r="V22" s="26"/>
       <c r="W22" s="25"/>
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
-      <c r="AA22" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AA22" s="26"/>
       <c r="AB22" s="26"/>
       <c r="AC22" s="26"/>
       <c r="AD22" s="26"/>
       <c r="AE22" s="26"/>
-      <c r="AF22" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="AF22" s="26"/>
       <c r="AG22" s="26"/>
       <c r="AH22" s="26"/>
       <c r="AI22" s="26"/>
-      <c r="AJ22" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AJ22" s="26"/>
       <c r="AK22" s="26"/>
       <c r="AL22" s="26"/>
       <c r="AM22" s="26"/>
@@ -30186,12 +30242,12 @@
       </c>
       <c r="BB22" s="5"/>
       <c r="BC22" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="32" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="26"/>
@@ -30200,18 +30256,14 @@
       <c r="F23" s="26"/>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
-      <c r="I23" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="I23" s="26"/>
       <c r="J23" s="26"/>
       <c r="K23" s="25"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
       <c r="O23" s="26"/>
-      <c r="P23" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
       <c r="R23" s="26"/>
       <c r="S23" s="26"/>
@@ -30219,12 +30271,12 @@
       <c r="U23" s="26"/>
       <c r="V23" s="26"/>
       <c r="W23" s="25"/>
-      <c r="X23" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="X23" s="26"/>
       <c r="Y23" s="26"/>
       <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
+      <c r="AA23" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AB23" s="26"/>
       <c r="AC23" s="26"/>
       <c r="AD23" s="26"/>
@@ -30235,10 +30287,10 @@
       <c r="AG23" s="26"/>
       <c r="AH23" s="26"/>
       <c r="AI23" s="26"/>
-      <c r="AJ23" s="26"/>
-      <c r="AK23" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AJ23" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="AK23" s="26"/>
       <c r="AL23" s="26"/>
       <c r="AM23" s="26"/>
       <c r="AN23" s="26"/>
@@ -30265,37 +30317,37 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="32" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
-      <c r="E24" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="E24" s="26"/>
       <c r="F24" s="26"/>
       <c r="G24" s="26"/>
-      <c r="H24" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="I24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="J24" s="26"/>
       <c r="K24" s="25"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
       <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
+      <c r="P24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="Q24" s="26"/>
-      <c r="R24" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="R24" s="26"/>
       <c r="S24" s="26"/>
       <c r="T24" s="26"/>
       <c r="U24" s="26"/>
       <c r="V24" s="26"/>
       <c r="W24" s="25"/>
-      <c r="X24" s="26"/>
+      <c r="X24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="Y24" s="26"/>
       <c r="Z24" s="26"/>
       <c r="AA24" s="26"/>
@@ -30303,12 +30355,16 @@
       <c r="AC24" s="26"/>
       <c r="AD24" s="26"/>
       <c r="AE24" s="26"/>
-      <c r="AF24" s="26"/>
+      <c r="AF24" s="26">
+        <v>3.0</v>
+      </c>
       <c r="AG24" s="26"/>
       <c r="AH24" s="26"/>
       <c r="AI24" s="26"/>
       <c r="AJ24" s="26"/>
-      <c r="AK24" s="26"/>
+      <c r="AK24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AL24" s="26"/>
       <c r="AM24" s="26"/>
       <c r="AN24" s="26"/>
@@ -30326,11 +30382,9 @@
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="BB24" s="5">
-        <v>2.0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="BB24" s="5"/>
       <c r="BC24" s="5">
         <v>1.0</v>
       </c>
@@ -30621,7 +30675,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
@@ -30951,7 +31005,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="25"/>
       <c r="C34" s="26"/>
@@ -31507,7 +31561,7 @@
       </c>
       <c r="AM40" s="5">
         <f>'League Table'!AM41</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AN40" s="5">
         <f>'League Table'!AN41</f>
@@ -31735,7 +31789,7 @@
       </c>
       <c r="AL42" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM42" s="6">
         <f t="shared" si="3"/>
@@ -62779,7 +62833,9 @@
       <c r="AL5" s="16">
         <v>1.0</v>
       </c>
-      <c r="AM5" s="16"/>
+      <c r="AM5" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AN5" s="16"/>
       <c r="AO5" s="16"/>
       <c r="AP5" s="16"/>
@@ -62794,7 +62850,7 @@
       <c r="AY5" s="16"/>
       <c r="BA5" s="39">
         <f t="shared" ref="BA5:BA37" si="1">SUM(B5:AY5)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
@@ -62894,7 +62950,7 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26">
@@ -63036,7 +63092,9 @@
       <c r="AL8" s="16">
         <v>1.0</v>
       </c>
-      <c r="AM8" s="16"/>
+      <c r="AM8" s="16">
+        <v>1.0</v>
+      </c>
       <c r="AN8" s="16"/>
       <c r="AO8" s="16"/>
       <c r="AP8" s="16"/>
@@ -63051,7 +63109,7 @@
       <c r="AY8" s="16"/>
       <c r="BA8" s="39">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -63109,7 +63167,9 @@
       <c r="AJ9" s="30"/>
       <c r="AK9" s="30"/>
       <c r="AL9" s="30"/>
-      <c r="AM9" s="30"/>
+      <c r="AM9" s="30">
+        <v>1.0</v>
+      </c>
       <c r="AN9" s="30"/>
       <c r="AO9" s="30"/>
       <c r="AP9" s="30"/>
@@ -63124,12 +63184,12 @@
       <c r="AY9" s="30"/>
       <c r="BA9" s="39">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -63204,7 +63264,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -63279,7 +63339,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
@@ -63352,7 +63412,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -63425,7 +63485,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
@@ -63602,7 +63662,9 @@
       <c r="AL16" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM16" s="26"/>
+      <c r="AM16" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN16" s="26"/>
       <c r="AO16" s="26"/>
       <c r="AP16" s="26"/>
@@ -63617,12 +63679,12 @@
       <c r="AY16" s="26"/>
       <c r="BA16" s="39">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="26">
@@ -63807,7 +63869,7 @@
     </row>
     <row r="20">
       <c r="A20" s="32" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -63929,7 +63991,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -64409,7 +64471,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
@@ -64527,7 +64589,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -64704,7 +64766,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
@@ -65192,7 +65254,7 @@
       </c>
       <c r="AM41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN41" s="5">
         <f t="shared" si="2"/>
@@ -65244,7 +65306,7 @@
       </c>
       <c r="BA41" s="39">
         <f>SUM(B41:AZ41)</f>
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -66417,7 +66479,7 @@
         <v>168</v>
       </c>
       <c r="N9" s="5">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="10">
@@ -66438,19 +66500,19 @@
       </c>
       <c r="G10" s="46"/>
       <c r="H10" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="I10" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="L10" s="5">
         <v>3.0</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N10" s="5">
         <v>7.0</v>
@@ -66467,14 +66529,14 @@
         <v>176</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E11" s="46" t="s">
         <v>167</v>
       </c>
       <c r="G11" s="46"/>
       <c r="H11" s="5" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="I11" s="5">
         <v>5.0</v>
@@ -66483,7 +66545,7 @@
         <v>177</v>
       </c>
       <c r="L11" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>150</v>
@@ -66510,7 +66572,7 @@
       </c>
       <c r="G12" s="46"/>
       <c r="H12" s="5" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="I12" s="5">
         <v>5.0</v>
@@ -66615,7 +66677,7 @@
         <v>177</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G15" s="46"/>
       <c r="H15" s="5" t="s">
@@ -66625,7 +66687,7 @@
         <v>4.0</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L15" s="5">
         <v>2.0</v>
@@ -66651,7 +66713,7 @@
         <v>184</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G16" s="46"/>
       <c r="H16" s="5" t="s">
@@ -66687,7 +66749,7 @@
         <v>157</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G17" s="46"/>
       <c r="H17" s="5" t="s">
@@ -66701,7 +66763,7 @@
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N17" s="5">
         <v>5.0</v>
@@ -66772,7 +66834,7 @@
         <v>177</v>
       </c>
       <c r="N19" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="20">
@@ -66793,7 +66855,7 @@
       </c>
       <c r="G20" s="46"/>
       <c r="H20" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I20" s="5">
         <v>2.0</v>
@@ -66891,7 +66953,7 @@
         <v>181</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G23" s="46"/>
       <c r="H23" s="5" t="s">
@@ -66955,7 +67017,7 @@
         <v>150</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G25" s="46"/>
       <c r="H25" s="5" t="s">
@@ -67019,7 +67081,7 @@
         <v>182</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G27" s="46"/>
       <c r="H27" s="5" t="s">
@@ -67081,7 +67143,9 @@
       <c r="E29" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>213</v>
+      </c>
       <c r="I29" s="5"/>
       <c r="K29" s="5"/>
       <c r="M29" s="5" t="s">
@@ -67096,7 +67160,7 @@
         <v>28.0</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C30" s="46" t="s">
         <v>190</v>
@@ -67122,10 +67186,10 @@
         <v>29.0</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D31" s="46" t="s">
         <v>156</v>
@@ -67151,7 +67215,7 @@
         <v>152</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D32" s="46" t="s">
         <v>145</v>
@@ -67174,7 +67238,7 @@
         <v>31.0</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C33" s="46" t="s">
         <v>187</v>
@@ -67188,7 +67252,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="M33" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N33" s="58">
         <v>1.0</v>
@@ -67199,7 +67263,7 @@
         <v>32.0</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C34" s="46" t="s">
         <v>194</v>
@@ -67224,7 +67288,7 @@
         <v>33.0</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C35" s="46" t="s">
         <v>170</v>
@@ -67237,15 +67301,19 @@
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
+      <c r="M35" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="N35" s="58">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="46">
         <v>34.0</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C36" s="46" t="s">
         <v>149</v>
@@ -67266,7 +67334,7 @@
         <v>35.0</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C37" s="46" t="s">
         <v>161</v>
@@ -67287,10 +67355,10 @@
         <v>36.0</v>
       </c>
       <c r="B38" s="46" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D38" s="46" t="s">
         <v>199</v>
@@ -67307,7 +67375,7 @@
         <v>37.0</v>
       </c>
       <c r="B39" s="46" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C39" s="46" t="s">
         <v>187</v>
@@ -67326,10 +67394,18 @@
       <c r="A40" s="46">
         <v>38.0</v>
       </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
+      <c r="B40" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="C40" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>168</v>
+      </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="N40" s="5"/>

</xml_diff>